<commit_message>
Fixed rounding problem, and output excel for temporal excel output
</commit_message>
<xml_diff>
--- a/sheets/input/Pegan_Cove_South_Pond.xlsx
+++ b/sheets/input/Pegan_Cove_South_Pond.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="0" windowWidth="21860" windowHeight="15500" tabRatio="790" activeTab="3"/>
+    <workbookView xWindow="2560" yWindow="0" windowWidth="16760" windowHeight="15500" tabRatio="790"/>
   </bookViews>
   <sheets>
     <sheet name="Sample_and_Time_Input" sheetId="1" r:id="rId1"/>
@@ -239,9 +239,6 @@
     <t>Disequilbrium factor of Particulate Organic Carbon (ony if Cwdo is unavaliable)</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>Fraction of Organic Carbon Content in Sediment (only if a organism eats sediment)</t>
   </si>
   <si>
@@ -509,6 +506,9 @@
   </si>
   <si>
     <t>1,1,2024</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -1519,18 +1519,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1541,6 +1529,18 @@
     <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="559">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -4989,8 +4989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5056,7 +5056,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -5064,7 +5064,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -5072,7 +5072,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -5086,7 +5086,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>70</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -5138,7 +5138,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="2"/>
@@ -5164,7 +5164,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="57" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="18"/>
@@ -5173,7 +5173,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -5236,7 +5236,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="28"/>
@@ -5262,14 +5262,14 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="57" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="18"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -5320,7 +5320,7 @@
         <v>10</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C22" s="6"/>
     </row>
@@ -5340,14 +5340,14 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="57" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="18"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -5398,7 +5398,7 @@
         <v>10</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C32" s="6"/>
     </row>
@@ -5416,30 +5416,30 @@
       <c r="B34" s="8"/>
       <c r="C34" s="6"/>
       <c r="E34" s="70" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="57" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="18"/>
-      <c r="E35" s="78" t="s">
+      <c r="E35" s="86" t="s">
+        <v>78</v>
+      </c>
+      <c r="F35" s="86" t="s">
         <v>79</v>
-      </c>
-      <c r="F35" s="78" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
-      <c r="E36" s="79"/>
-      <c r="F36" s="79"/>
+      <c r="E36" s="87"/>
+      <c r="F36" s="87"/>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="7" t="s">
@@ -5449,11 +5449,11 @@
         <v>0.9</v>
       </c>
       <c r="C37" s="6"/>
-      <c r="E37" s="76" t="s">
+      <c r="E37" s="88" t="s">
+        <v>80</v>
+      </c>
+      <c r="F37" s="88" t="s">
         <v>81</v>
-      </c>
-      <c r="F37" s="76" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -5462,8 +5462,8 @@
       </c>
       <c r="B38" s="18"/>
       <c r="C38" s="6"/>
-      <c r="E38" s="77"/>
-      <c r="F38" s="77"/>
+      <c r="E38" s="89"/>
+      <c r="F38" s="89"/>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="7" t="s">
@@ -5471,11 +5471,11 @@
       </c>
       <c r="B39" s="18"/>
       <c r="C39" s="6"/>
-      <c r="E39" s="76" t="s">
+      <c r="E39" s="88" t="s">
+        <v>82</v>
+      </c>
+      <c r="F39" s="88" t="s">
         <v>83</v>
-      </c>
-      <c r="F39" s="76" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -5484,87 +5484,81 @@
       </c>
       <c r="B40" s="18"/>
       <c r="C40" s="6"/>
-      <c r="E40" s="77"/>
-      <c r="F40" s="77"/>
+      <c r="E40" s="89"/>
+      <c r="F40" s="89"/>
     </row>
     <row r="41" spans="1:6">
-      <c r="E41" s="76" t="s">
+      <c r="E41" s="88" t="s">
+        <v>84</v>
+      </c>
+      <c r="F41" s="88" t="s">
         <v>85</v>
       </c>
-      <c r="F41" s="76" t="s">
+    </row>
+    <row r="42" spans="1:6">
+      <c r="E42" s="89"/>
+      <c r="F42" s="89"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="E43" s="88" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="E42" s="77"/>
-      <c r="F42" s="77"/>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="E43" s="76" t="s">
+      <c r="F43" s="88" t="s">
         <v>87</v>
       </c>
-      <c r="F43" s="76" t="s">
+    </row>
+    <row r="44" spans="1:6">
+      <c r="E44" s="89"/>
+      <c r="F44" s="89"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="E45" s="88" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="E44" s="77"/>
-      <c r="F44" s="77"/>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="E45" s="76" t="s">
+      <c r="F45" s="88" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="E46" s="89"/>
+      <c r="F46" s="89"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="E47" s="88" t="s">
         <v>89</v>
       </c>
-      <c r="F45" s="76" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="E46" s="77"/>
-      <c r="F46" s="77"/>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="E47" s="76" t="s">
+      <c r="F47" s="88" t="s">
         <v>90</v>
       </c>
-      <c r="F47" s="76" t="s">
+    </row>
+    <row r="48" spans="1:6">
+      <c r="E48" s="89"/>
+      <c r="F48" s="89"/>
+    </row>
+    <row r="49" spans="5:6">
+      <c r="E49" s="88" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="E48" s="77"/>
-      <c r="F48" s="77"/>
-    </row>
-    <row r="49" spans="5:6">
-      <c r="E49" s="76" t="s">
+      <c r="F49" s="88" t="s">
         <v>92</v>
       </c>
-      <c r="F49" s="76" t="s">
-        <v>93</v>
-      </c>
     </row>
     <row r="50" spans="5:6">
-      <c r="E50" s="77"/>
-      <c r="F50" s="77"/>
+      <c r="E50" s="89"/>
+      <c r="F50" s="89"/>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="71" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="5:6" ht="28" customHeight="1">
       <c r="E53" s="71" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
     <mergeCell ref="E47:E48"/>
     <mergeCell ref="F47:F48"/>
     <mergeCell ref="E49:E50"/>
@@ -5575,6 +5569,12 @@
     <mergeCell ref="F43:F44"/>
     <mergeCell ref="E45:E46"/>
     <mergeCell ref="F45:F46"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5619,147 +5619,147 @@
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E1" s="13"/>
       <c r="F1" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G1" s="13"/>
       <c r="H1" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I1" s="13"/>
       <c r="J1" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K1" s="13"/>
       <c r="L1" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M1" s="13"/>
       <c r="N1" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O1" s="13"/>
       <c r="P1" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q1" s="13"/>
       <c r="R1" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S1" s="13"/>
       <c r="T1" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U1" s="13"/>
       <c r="V1" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="W1" s="13"/>
       <c r="X1" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Y1" s="13"/>
       <c r="Z1" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AA1" s="13"/>
       <c r="AB1" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AC1" s="13"/>
       <c r="AD1" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AE1" s="13"/>
       <c r="AF1" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AG1" s="13"/>
       <c r="AH1" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AI1" s="13"/>
       <c r="AJ1" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AK1" s="13"/>
       <c r="AL1" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AM1" s="13"/>
       <c r="AN1" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AO1" s="13"/>
       <c r="AP1" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AQ1" s="13"/>
       <c r="AR1" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AS1" s="13"/>
       <c r="AT1" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AU1" s="13"/>
       <c r="AV1" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AW1" s="13"/>
       <c r="AX1" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AY1" s="13"/>
       <c r="AZ1" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="BA1" s="13"/>
       <c r="BB1" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="BC1" s="13"/>
       <c r="BD1" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="BE1" s="13"/>
       <c r="BF1" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="BG1" s="13"/>
       <c r="BH1" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="BI1" s="13"/>
       <c r="BJ1" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BK1" s="13"/>
       <c r="BL1" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BM1" s="13"/>
       <c r="BN1" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="BO1" s="13"/>
       <c r="BP1" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="BQ1" s="13"/>
       <c r="BR1" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="BS1" s="13"/>
       <c r="BT1" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="BU1" s="13"/>
       <c r="BV1" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="BW1" s="13"/>
     </row>
@@ -5990,7 +5990,7 @@
     </row>
     <row r="3" spans="1:75">
       <c r="A3" s="72" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" s="15">
         <v>8</v>
@@ -6368,7 +6368,7 @@
     </row>
     <row r="5" spans="1:75">
       <c r="A5" s="72" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5" s="15">
         <v>8</v>
@@ -6520,760 +6520,760 @@
       <c r="BW5" s="16"/>
     </row>
     <row r="6" spans="1:75">
-      <c r="A6" s="84"/>
-      <c r="B6" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="86" t="s">
+      <c r="A6" s="80"/>
+      <c r="B6" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="82" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="86" t="s">
+      <c r="E6" s="82" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="86" t="s">
+      <c r="G6" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="82" t="s">
         <v>9</v>
       </c>
       <c r="L6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="86" t="s">
+      <c r="M6" s="82" t="s">
         <v>9</v>
       </c>
       <c r="N6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="P6" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q6" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="R6" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="S6" s="86" t="s">
+      <c r="O6" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q6" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="R6" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="S6" s="82" t="s">
         <v>9</v>
       </c>
       <c r="T6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="U6" s="86" t="s">
+      <c r="U6" s="82" t="s">
         <v>9</v>
       </c>
       <c r="V6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="W6" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="X6" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y6" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z6" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA6" s="86" t="s">
+      <c r="W6" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="X6" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y6" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z6" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA6" s="82" t="s">
         <v>9</v>
       </c>
       <c r="AB6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AC6" s="86" t="s">
+      <c r="AC6" s="82" t="s">
         <v>9</v>
       </c>
       <c r="AD6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AE6" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF6" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG6" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH6" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI6" s="86" t="s">
+      <c r="AE6" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF6" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG6" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH6" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI6" s="82" t="s">
         <v>9</v>
       </c>
       <c r="AJ6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AK6" s="86" t="s">
+      <c r="AK6" s="82" t="s">
         <v>9</v>
       </c>
       <c r="AL6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AM6" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="AN6" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="AO6" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="AP6" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="AQ6" s="86" t="s">
+      <c r="AM6" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="AN6" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO6" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="AP6" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ6" s="82" t="s">
         <v>9</v>
       </c>
       <c r="AR6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AS6" s="86" t="s">
+      <c r="AS6" s="82" t="s">
         <v>9</v>
       </c>
       <c r="AT6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AU6" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="AV6" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="AW6" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="AX6" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="AY6" s="86" t="s">
+      <c r="AU6" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="AV6" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW6" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="AX6" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="AY6" s="82" t="s">
         <v>9</v>
       </c>
       <c r="AZ6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BA6" s="86" t="s">
+      <c r="BA6" s="82" t="s">
         <v>9</v>
       </c>
       <c r="BB6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BC6" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="BD6" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="BE6" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="BF6" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="BG6" s="86" t="s">
+      <c r="BC6" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="BD6" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="BE6" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="BF6" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="BG6" s="82" t="s">
         <v>9</v>
       </c>
       <c r="BH6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BI6" s="86" t="s">
+      <c r="BI6" s="82" t="s">
         <v>9</v>
       </c>
       <c r="BJ6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BK6" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="BL6" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="BM6" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="BN6" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="BO6" s="86" t="s">
+      <c r="BK6" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="BL6" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="BM6" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="BN6" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="BO6" s="82" t="s">
         <v>9</v>
       </c>
       <c r="BP6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BQ6" s="86" t="s">
+      <c r="BQ6" s="82" t="s">
         <v>9</v>
       </c>
       <c r="BR6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BS6" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="BT6" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="BU6" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="BV6" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="BW6" s="86" t="s">
+      <c r="BS6" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="BT6" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="BU6" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="BV6" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="BW6" s="82" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:75">
-      <c r="A7" s="87" t="s">
-        <v>102</v>
-      </c>
-      <c r="B7" s="88">
+      <c r="A7" s="83" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="84">
         <v>8</v>
       </c>
-      <c r="C7" s="89"/>
+      <c r="C7" s="85"/>
       <c r="D7" s="69">
         <v>13</v>
       </c>
-      <c r="E7" s="89"/>
+      <c r="E7" s="85"/>
       <c r="F7" s="69">
         <v>18</v>
       </c>
-      <c r="G7" s="89"/>
+      <c r="G7" s="85"/>
       <c r="H7" s="69">
         <v>13</v>
       </c>
-      <c r="I7" s="89"/>
-      <c r="J7" s="88">
+      <c r="I7" s="85"/>
+      <c r="J7" s="84">
         <v>8</v>
       </c>
-      <c r="K7" s="89"/>
+      <c r="K7" s="85"/>
       <c r="L7" s="69">
         <v>13</v>
       </c>
-      <c r="M7" s="89"/>
+      <c r="M7" s="85"/>
       <c r="N7" s="69">
         <v>18</v>
       </c>
-      <c r="O7" s="89"/>
+      <c r="O7" s="85"/>
       <c r="P7" s="69">
         <v>13</v>
       </c>
-      <c r="Q7" s="89"/>
-      <c r="R7" s="88">
+      <c r="Q7" s="85"/>
+      <c r="R7" s="84">
         <v>8</v>
       </c>
-      <c r="S7" s="89"/>
+      <c r="S7" s="85"/>
       <c r="T7" s="69">
         <v>13</v>
       </c>
-      <c r="U7" s="89"/>
+      <c r="U7" s="85"/>
       <c r="V7" s="69">
         <v>18</v>
       </c>
-      <c r="W7" s="89"/>
+      <c r="W7" s="85"/>
       <c r="X7" s="69">
         <v>13</v>
       </c>
-      <c r="Y7" s="89"/>
-      <c r="Z7" s="88">
+      <c r="Y7" s="85"/>
+      <c r="Z7" s="84">
         <v>8</v>
       </c>
-      <c r="AA7" s="89"/>
+      <c r="AA7" s="85"/>
       <c r="AB7" s="69">
         <v>13</v>
       </c>
-      <c r="AC7" s="89"/>
+      <c r="AC7" s="85"/>
       <c r="AD7" s="69">
         <v>18</v>
       </c>
-      <c r="AE7" s="89"/>
+      <c r="AE7" s="85"/>
       <c r="AF7" s="69">
         <v>13</v>
       </c>
-      <c r="AG7" s="89"/>
-      <c r="AH7" s="88">
+      <c r="AG7" s="85"/>
+      <c r="AH7" s="84">
         <v>8</v>
       </c>
-      <c r="AI7" s="89"/>
+      <c r="AI7" s="85"/>
       <c r="AJ7" s="69">
         <v>13</v>
       </c>
-      <c r="AK7" s="89"/>
+      <c r="AK7" s="85"/>
       <c r="AL7" s="69">
         <v>18</v>
       </c>
-      <c r="AM7" s="89"/>
+      <c r="AM7" s="85"/>
       <c r="AN7" s="69">
         <v>13</v>
       </c>
-      <c r="AO7" s="89"/>
-      <c r="AP7" s="88">
+      <c r="AO7" s="85"/>
+      <c r="AP7" s="84">
         <v>8</v>
       </c>
-      <c r="AQ7" s="89"/>
+      <c r="AQ7" s="85"/>
       <c r="AR7" s="69">
         <v>13</v>
       </c>
-      <c r="AS7" s="89"/>
+      <c r="AS7" s="85"/>
       <c r="AT7" s="69">
         <v>18</v>
       </c>
-      <c r="AU7" s="89"/>
+      <c r="AU7" s="85"/>
       <c r="AV7" s="69">
         <v>13</v>
       </c>
-      <c r="AW7" s="89"/>
-      <c r="AX7" s="88">
+      <c r="AW7" s="85"/>
+      <c r="AX7" s="84">
         <v>8</v>
       </c>
-      <c r="AY7" s="89"/>
+      <c r="AY7" s="85"/>
       <c r="AZ7" s="69">
         <v>13</v>
       </c>
-      <c r="BA7" s="89"/>
+      <c r="BA7" s="85"/>
       <c r="BB7" s="69">
         <v>18</v>
       </c>
-      <c r="BC7" s="89"/>
+      <c r="BC7" s="85"/>
       <c r="BD7" s="69">
         <v>13</v>
       </c>
-      <c r="BE7" s="89"/>
-      <c r="BF7" s="88">
+      <c r="BE7" s="85"/>
+      <c r="BF7" s="84">
         <v>8</v>
       </c>
-      <c r="BG7" s="89"/>
+      <c r="BG7" s="85"/>
       <c r="BH7" s="69">
         <v>13</v>
       </c>
-      <c r="BI7" s="89"/>
+      <c r="BI7" s="85"/>
       <c r="BJ7" s="69">
         <v>18</v>
       </c>
-      <c r="BK7" s="89"/>
+      <c r="BK7" s="85"/>
       <c r="BL7" s="69">
         <v>13</v>
       </c>
-      <c r="BM7" s="89"/>
-      <c r="BN7" s="88">
+      <c r="BM7" s="85"/>
+      <c r="BN7" s="84">
         <v>8</v>
       </c>
-      <c r="BO7" s="89"/>
+      <c r="BO7" s="85"/>
       <c r="BP7" s="69">
         <v>13</v>
       </c>
-      <c r="BQ7" s="89"/>
+      <c r="BQ7" s="85"/>
       <c r="BR7" s="69">
         <v>18</v>
       </c>
-      <c r="BS7" s="89"/>
+      <c r="BS7" s="85"/>
       <c r="BT7" s="69">
         <v>13</v>
       </c>
-      <c r="BU7" s="89"/>
-      <c r="BV7" s="88">
+      <c r="BU7" s="85"/>
+      <c r="BV7" s="84">
         <v>8</v>
       </c>
-      <c r="BW7" s="89"/>
+      <c r="BW7" s="85"/>
     </row>
     <row r="8" spans="1:75">
-      <c r="A8" s="84"/>
-      <c r="B8" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="86" t="s">
+      <c r="A8" s="80"/>
+      <c r="B8" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="82" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="86" t="s">
+      <c r="E8" s="82" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="86" t="s">
+      <c r="G8" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="82" t="s">
         <v>9</v>
       </c>
       <c r="L8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="M8" s="86" t="s">
+      <c r="M8" s="82" t="s">
         <v>9</v>
       </c>
       <c r="N8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="O8" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="P8" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q8" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="R8" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="S8" s="86" t="s">
+      <c r="O8" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="P8" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q8" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="R8" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="S8" s="82" t="s">
         <v>9</v>
       </c>
       <c r="T8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="U8" s="86" t="s">
+      <c r="U8" s="82" t="s">
         <v>9</v>
       </c>
       <c r="V8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="W8" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="X8" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y8" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z8" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA8" s="86" t="s">
+      <c r="W8" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="X8" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y8" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z8" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA8" s="82" t="s">
         <v>9</v>
       </c>
       <c r="AB8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AC8" s="86" t="s">
+      <c r="AC8" s="82" t="s">
         <v>9</v>
       </c>
       <c r="AD8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AE8" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF8" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG8" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH8" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI8" s="86" t="s">
+      <c r="AE8" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF8" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG8" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH8" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI8" s="82" t="s">
         <v>9</v>
       </c>
       <c r="AJ8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AK8" s="86" t="s">
+      <c r="AK8" s="82" t="s">
         <v>9</v>
       </c>
       <c r="AL8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AM8" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="AN8" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="AO8" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="AP8" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="AQ8" s="86" t="s">
+      <c r="AM8" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="AN8" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO8" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="AP8" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ8" s="82" t="s">
         <v>9</v>
       </c>
       <c r="AR8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AS8" s="86" t="s">
+      <c r="AS8" s="82" t="s">
         <v>9</v>
       </c>
       <c r="AT8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AU8" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="AV8" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="AW8" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="AX8" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="AY8" s="86" t="s">
+      <c r="AU8" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="AV8" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW8" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="AX8" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="AY8" s="82" t="s">
         <v>9</v>
       </c>
       <c r="AZ8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BA8" s="86" t="s">
+      <c r="BA8" s="82" t="s">
         <v>9</v>
       </c>
       <c r="BB8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BC8" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="BD8" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="BE8" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="BF8" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="BG8" s="86" t="s">
+      <c r="BC8" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="BD8" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="BE8" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="BF8" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="BG8" s="82" t="s">
         <v>9</v>
       </c>
       <c r="BH8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BI8" s="86" t="s">
+      <c r="BI8" s="82" t="s">
         <v>9</v>
       </c>
       <c r="BJ8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BK8" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="BL8" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="BM8" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="BN8" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="BO8" s="86" t="s">
+      <c r="BK8" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="BL8" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="BM8" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="BN8" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="BO8" s="82" t="s">
         <v>9</v>
       </c>
       <c r="BP8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BQ8" s="86" t="s">
+      <c r="BQ8" s="82" t="s">
         <v>9</v>
       </c>
       <c r="BR8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BS8" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="BT8" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="BU8" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="BV8" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="BW8" s="86" t="s">
+      <c r="BS8" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="BT8" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="BU8" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="BV8" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="BW8" s="82" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:75">
-      <c r="A9" s="87" t="s">
-        <v>102</v>
-      </c>
-      <c r="B9" s="88">
+      <c r="A9" s="83" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="84">
         <v>8</v>
       </c>
-      <c r="C9" s="89"/>
+      <c r="C9" s="85"/>
       <c r="D9" s="69">
         <v>13</v>
       </c>
-      <c r="E9" s="89"/>
+      <c r="E9" s="85"/>
       <c r="F9" s="69">
         <v>18</v>
       </c>
-      <c r="G9" s="89"/>
+      <c r="G9" s="85"/>
       <c r="H9" s="69">
         <v>13</v>
       </c>
-      <c r="I9" s="89"/>
-      <c r="J9" s="88">
+      <c r="I9" s="85"/>
+      <c r="J9" s="84">
         <v>8</v>
       </c>
-      <c r="K9" s="89"/>
+      <c r="K9" s="85"/>
       <c r="L9" s="69">
         <v>13</v>
       </c>
-      <c r="M9" s="89"/>
+      <c r="M9" s="85"/>
       <c r="N9" s="69">
         <v>18</v>
       </c>
-      <c r="O9" s="89"/>
+      <c r="O9" s="85"/>
       <c r="P9" s="69">
         <v>13</v>
       </c>
-      <c r="Q9" s="89"/>
-      <c r="R9" s="88">
+      <c r="Q9" s="85"/>
+      <c r="R9" s="84">
         <v>8</v>
       </c>
-      <c r="S9" s="89"/>
+      <c r="S9" s="85"/>
       <c r="T9" s="69">
         <v>13</v>
       </c>
-      <c r="U9" s="89"/>
+      <c r="U9" s="85"/>
       <c r="V9" s="69">
         <v>18</v>
       </c>
-      <c r="W9" s="89"/>
+      <c r="W9" s="85"/>
       <c r="X9" s="69">
         <v>13</v>
       </c>
-      <c r="Y9" s="89"/>
-      <c r="Z9" s="88">
+      <c r="Y9" s="85"/>
+      <c r="Z9" s="84">
         <v>8</v>
       </c>
-      <c r="AA9" s="89"/>
+      <c r="AA9" s="85"/>
       <c r="AB9" s="69">
         <v>13</v>
       </c>
-      <c r="AC9" s="89"/>
+      <c r="AC9" s="85"/>
       <c r="AD9" s="69">
         <v>18</v>
       </c>
-      <c r="AE9" s="89"/>
+      <c r="AE9" s="85"/>
       <c r="AF9" s="69">
         <v>13</v>
       </c>
-      <c r="AG9" s="89"/>
-      <c r="AH9" s="88">
+      <c r="AG9" s="85"/>
+      <c r="AH9" s="84">
         <v>8</v>
       </c>
-      <c r="AI9" s="89"/>
+      <c r="AI9" s="85"/>
       <c r="AJ9" s="69">
         <v>13</v>
       </c>
-      <c r="AK9" s="89"/>
+      <c r="AK9" s="85"/>
       <c r="AL9" s="69">
         <v>18</v>
       </c>
-      <c r="AM9" s="89"/>
+      <c r="AM9" s="85"/>
       <c r="AN9" s="69">
         <v>13</v>
       </c>
-      <c r="AO9" s="89"/>
-      <c r="AP9" s="88">
+      <c r="AO9" s="85"/>
+      <c r="AP9" s="84">
         <v>8</v>
       </c>
-      <c r="AQ9" s="89"/>
+      <c r="AQ9" s="85"/>
       <c r="AR9" s="69">
         <v>13</v>
       </c>
-      <c r="AS9" s="89"/>
+      <c r="AS9" s="85"/>
       <c r="AT9" s="69">
         <v>18</v>
       </c>
-      <c r="AU9" s="89"/>
+      <c r="AU9" s="85"/>
       <c r="AV9" s="69">
         <v>13</v>
       </c>
-      <c r="AW9" s="89"/>
-      <c r="AX9" s="88">
+      <c r="AW9" s="85"/>
+      <c r="AX9" s="84">
         <v>8</v>
       </c>
-      <c r="AY9" s="89"/>
+      <c r="AY9" s="85"/>
       <c r="AZ9" s="69">
         <v>13</v>
       </c>
-      <c r="BA9" s="89"/>
+      <c r="BA9" s="85"/>
       <c r="BB9" s="69">
         <v>18</v>
       </c>
-      <c r="BC9" s="89"/>
+      <c r="BC9" s="85"/>
       <c r="BD9" s="69">
         <v>13</v>
       </c>
-      <c r="BE9" s="89"/>
-      <c r="BF9" s="88">
+      <c r="BE9" s="85"/>
+      <c r="BF9" s="84">
         <v>8</v>
       </c>
-      <c r="BG9" s="89"/>
+      <c r="BG9" s="85"/>
       <c r="BH9" s="69">
         <v>13</v>
       </c>
-      <c r="BI9" s="89"/>
+      <c r="BI9" s="85"/>
       <c r="BJ9" s="69">
         <v>18</v>
       </c>
-      <c r="BK9" s="89"/>
+      <c r="BK9" s="85"/>
       <c r="BL9" s="69">
         <v>13</v>
       </c>
-      <c r="BM9" s="89"/>
-      <c r="BN9" s="88">
+      <c r="BM9" s="85"/>
+      <c r="BN9" s="84">
         <v>8</v>
       </c>
-      <c r="BO9" s="89"/>
+      <c r="BO9" s="85"/>
       <c r="BP9" s="69">
         <v>13</v>
       </c>
-      <c r="BQ9" s="89"/>
+      <c r="BQ9" s="85"/>
       <c r="BR9" s="69">
         <v>18</v>
       </c>
-      <c r="BS9" s="89"/>
+      <c r="BS9" s="85"/>
       <c r="BT9" s="69">
         <v>13</v>
       </c>
-      <c r="BU9" s="89"/>
-      <c r="BV9" s="88">
+      <c r="BU9" s="85"/>
+      <c r="BV9" s="84">
         <v>8</v>
       </c>
-      <c r="BW9" s="89"/>
+      <c r="BW9" s="85"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7291,7 +7291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -7330,7 +7330,7 @@
         <v>18</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="28"/>
@@ -7403,7 +7403,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="42">
         <v>2.2400000000000002</v>
@@ -7423,7 +7423,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="69" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" s="43">
         <v>0.1</v>
@@ -7443,7 +7443,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B8" s="42"/>
       <c r="C8" s="6"/>
@@ -7461,7 +7461,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B9" s="42"/>
       <c r="C9" s="42"/>
@@ -7478,9 +7478,9 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="B10" s="83">
+        <v>144</v>
+      </c>
+      <c r="B10" s="79">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="C10" s="6"/>
@@ -7497,7 +7497,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B11" s="8">
         <v>2.65E-5</v>
@@ -7516,7 +7516,7 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B12" s="42"/>
       <c r="C12" s="6"/>
@@ -7533,7 +7533,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B13" s="42"/>
       <c r="C13" s="42"/>
@@ -7551,16 +7551,16 @@
     </row>
     <row r="14" spans="1:14" ht="18" customHeight="1">
       <c r="A14" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="B14" s="83">
+        <v>147</v>
+      </c>
+      <c r="B14" s="79">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B15" s="8">
         <v>2.65E-5</v>
@@ -7569,19 +7569,19 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B16" s="42"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B17" s="42"/>
     </row>
     <row r="18" spans="1:3" ht="17" customHeight="1">
       <c r="A18" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B18" s="8">
         <v>6.3999999999999997E-6</v>
@@ -7589,7 +7589,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B19" s="8">
         <v>1.2500000000000001E-5</v>
@@ -7597,21 +7597,21 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B20" s="42"/>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B21" s="42"/>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B22" s="8">
         <v>6.3999999999999997E-6</v>
@@ -7620,7 +7620,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B23" s="8">
         <v>1.2500000000000001E-5</v>
@@ -7707,8 +7707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7734,7 +7734,7 @@
       <c r="B1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="76" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="20" t="s">
@@ -7746,7 +7746,7 @@
       <c r="F1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="82" t="s">
+      <c r="G1" s="78" t="s">
         <v>20</v>
       </c>
       <c r="H1" s="20" t="s">
@@ -7770,7 +7770,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="23" t="s">
@@ -7795,7 +7795,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" s="6">
         <v>4.7E-2</v>
@@ -7814,7 +7814,7 @@
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K3" s="36">
         <v>0.08</v>
@@ -7863,7 +7863,9 @@
       <c r="G5" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="25"/>
+      <c r="H5" s="25">
+        <v>4.7E-2</v>
+      </c>
       <c r="I5" s="6"/>
       <c r="J5" s="9" t="s">
         <v>27</v>
@@ -7992,7 +7994,7 @@
         <v>34</v>
       </c>
       <c r="B12" s="10"/>
-      <c r="C12" s="81"/>
+      <c r="C12" s="77"/>
       <c r="D12" s="31" t="s">
         <v>34</v>
       </c>
@@ -8031,7 +8033,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="2"/>
@@ -8040,7 +8042,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B15" s="6">
         <v>9.8000000000000004E-2</v>
@@ -8158,13 +8160,13 @@
         <v>10</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C26" s="6"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B27" s="6">
         <v>0.43099999999999999</v>
@@ -8281,7 +8283,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="53" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2" s="53"/>
     </row>
@@ -8311,7 +8313,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="53" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" s="53">
         <v>0</v>
@@ -8319,7 +8321,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="53" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B7" s="53">
         <v>0</v>
@@ -8330,7 +8332,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="53" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B8" s="53">
         <v>0</v>
@@ -8346,7 +8348,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="53" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B10" s="53"/>
     </row>
@@ -8376,7 +8378,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="53" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B14" s="53">
         <v>0</v>
@@ -8384,7 +8386,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="53" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B15" s="53">
         <v>0</v>
@@ -8392,7 +8394,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="53" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B16" s="53">
         <v>0</v>
@@ -8411,7 +8413,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="53" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B18" s="53"/>
     </row>
@@ -8441,7 +8443,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="53" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B22" s="53">
         <v>0.7</v>
@@ -8449,7 +8451,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="53" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B23" s="53">
         <v>0</v>
@@ -8460,7 +8462,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="53" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B24" s="53">
         <v>0</v>
@@ -8549,34 +8551,34 @@
         <v>63</v>
       </c>
       <c r="E1" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="G1" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="G1" s="44" t="s">
+      <c r="H1" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="H1" s="44" t="s">
+      <c r="I1" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="I1" s="44" t="s">
+      <c r="J1" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="J1" s="44" t="s">
-        <v>123</v>
-      </c>
       <c r="K1" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="L1" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="L1" s="44" t="s">
+      <c r="M1" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="M1" s="44" t="s">
+      <c r="N1" s="44" t="s">
         <v>122</v>
-      </c>
-      <c r="N1" s="44" t="s">
-        <v>123</v>
       </c>
       <c r="O1" s="44" t="s">
         <v>38</v>
@@ -8588,34 +8590,34 @@
         <v>63</v>
       </c>
       <c r="R1" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="S1" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="S1" s="44" t="s">
+      <c r="T1" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="T1" s="44" t="s">
+      <c r="U1" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="U1" s="44" t="s">
+      <c r="V1" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="V1" s="44" t="s">
+      <c r="W1" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="W1" s="44" t="s">
-        <v>123</v>
-      </c>
       <c r="X1" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y1" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="Y1" s="44" t="s">
+      <c r="Z1" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="Z1" s="44" t="s">
+      <c r="AA1" s="44" t="s">
         <v>122</v>
-      </c>
-      <c r="AA1" s="44" t="s">
-        <v>123</v>
       </c>
       <c r="AB1" s="44" t="s">
         <v>38</v>
@@ -8627,34 +8629,34 @@
         <v>63</v>
       </c>
       <c r="AE1" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF1" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="AF1" s="44" t="s">
+      <c r="AG1" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="AG1" s="44" t="s">
+      <c r="AH1" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="AH1" s="44" t="s">
+      <c r="AI1" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="AI1" s="44" t="s">
+      <c r="AJ1" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="AJ1" s="44" t="s">
-        <v>123</v>
-      </c>
       <c r="AK1" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="AL1" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="AL1" s="44" t="s">
+      <c r="AM1" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="AM1" s="44" t="s">
+      <c r="AN1" s="44" t="s">
         <v>122</v>
-      </c>
-      <c r="AN1" s="44" t="s">
-        <v>123</v>
       </c>
       <c r="AO1" s="44" t="s">
         <v>38</v>
@@ -8666,34 +8668,34 @@
         <v>63</v>
       </c>
       <c r="AR1" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS1" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="AS1" s="44" t="s">
+      <c r="AT1" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="AT1" s="44" t="s">
+      <c r="AU1" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="AU1" s="44" t="s">
+      <c r="AV1" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="AV1" s="44" t="s">
+      <c r="AW1" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="AW1" s="44" t="s">
-        <v>123</v>
-      </c>
       <c r="AX1" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="AY1" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="AY1" s="44" t="s">
+      <c r="AZ1" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="AZ1" s="44" t="s">
+      <c r="BA1" s="44" t="s">
         <v>122</v>
-      </c>
-      <c r="BA1" s="44" t="s">
-        <v>123</v>
       </c>
       <c r="BB1" s="17"/>
       <c r="BC1" s="17"/>
@@ -9177,7 +9179,7 @@
     </row>
     <row r="2" spans="1:532">
       <c r="A2" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2" s="45">
         <v>1</v>
@@ -9342,7 +9344,7 @@
     </row>
     <row r="3" spans="1:532">
       <c r="A3" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B3" s="45">
         <v>1</v>
@@ -9507,7 +9509,7 @@
     </row>
     <row r="4" spans="1:532">
       <c r="A4" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" s="45">
         <v>1</v>
@@ -9727,13 +9729,13 @@
         <v>45</v>
       </c>
       <c r="C2" s="47" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="E2" s="47" t="s">
         <v>125</v>
-      </c>
-      <c r="E2" s="47" t="s">
-        <v>126</v>
       </c>
       <c r="F2" s="17"/>
       <c r="G2" s="17"/>
@@ -9758,10 +9760,10 @@
     <row r="4" spans="1:8">
       <c r="A4" s="48"/>
       <c r="B4" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
@@ -9772,10 +9774,10 @@
     <row r="5" spans="1:8">
       <c r="A5" s="48"/>
       <c r="B5" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -9786,10 +9788,10 @@
     <row r="6" spans="1:8">
       <c r="A6" s="48"/>
       <c r="B6" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
@@ -9800,10 +9802,10 @@
     <row r="7" spans="1:8">
       <c r="A7" s="48"/>
       <c r="B7" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
@@ -10141,13 +10143,13 @@
     </row>
     <row r="40" spans="1:49">
       <c r="A40" s="45" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B40" s="45" t="s">
         <v>49</v>
       </c>
       <c r="C40" s="45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D40" s="51" t="s">
         <v>52</v>
@@ -10165,10 +10167,10 @@
     </row>
     <row r="41" spans="1:49">
       <c r="A41" s="45" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B41" s="45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C41" s="45">
         <v>1</v>
@@ -10177,13 +10179,13 @@
         <v>45</v>
       </c>
       <c r="E41" s="45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F41" s="45" t="s">
         <v>56</v>
       </c>
       <c r="G41" s="45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H41" s="17"/>
       <c r="AW41" t="s">
@@ -10192,10 +10194,10 @@
     </row>
     <row r="42" spans="1:49">
       <c r="A42" s="45" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B42" s="46" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C42" s="45">
         <v>1</v>
@@ -10204,13 +10206,13 @@
         <v>45</v>
       </c>
       <c r="E42" s="45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F42" s="45" t="s">
         <v>56</v>
       </c>
       <c r="G42" s="45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H42" s="17"/>
       <c r="AW42" t="s">
@@ -10219,10 +10221,10 @@
     </row>
     <row r="43" spans="1:49">
       <c r="A43" s="46" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B43" s="46" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C43" s="46">
         <v>1</v>
@@ -10231,13 +10233,13 @@
         <v>45</v>
       </c>
       <c r="E43" s="45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F43" s="45" t="s">
         <v>56</v>
       </c>
       <c r="G43" s="45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AW43" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
cleaned a little bit
</commit_message>
<xml_diff>
--- a/sheets/input/Pegan_Cove_South_Pond.xlsx
+++ b/sheets/input/Pegan_Cove_South_Pond.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="0" windowWidth="16760" windowHeight="15500" tabRatio="790"/>
+    <workbookView xWindow="2560" yWindow="0" windowWidth="22580" windowHeight="16260" tabRatio="790" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sample_and_Time_Input" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="160">
   <si>
     <t>Number of Hyper-cube bins</t>
   </si>
@@ -240,12 +240,6 @@
   </si>
   <si>
     <t>Fraction of Organic Carbon Content in Sediment (only if a organism eats sediment)</t>
-  </si>
-  <si>
-    <t>beta_lip (defualt = 1)</t>
-  </si>
-  <si>
-    <t>beta_prot (defualt = .35)</t>
   </si>
   <si>
     <t>0,10</t>
@@ -475,9 +469,6 @@
     <t xml:space="preserve">Dissolved Concentration in Water at Pegan Cove (ug/L) </t>
   </si>
   <si>
-    <t>Concentration in Pour Water at Pegan Cove (ug/L)</t>
-  </si>
-  <si>
     <t>Total Concentration in Water at Pegan Cove dummy (only if Cwdo is unavaliable) (ug/L)</t>
   </si>
   <si>
@@ -509,6 +500,24 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Beta Lipid Omn (default = 1)</t>
+  </si>
+  <si>
+    <t>Beta Non-lipid OM (defualt = 0.035)</t>
+  </si>
+  <si>
+    <t>Beta Lipid digesta (default = 1)</t>
+  </si>
+  <si>
+    <t>Beta Sediment OC (default = .35)</t>
+  </si>
+  <si>
+    <t>Beta  Non-lipid digesta  (defualt = .035)</t>
+  </si>
+  <si>
+    <t>Concentration in Pore Water at Pegan Cove (ug/L)</t>
   </si>
 </sst>
 </file>
@@ -1430,7 +1439,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1522,24 +1531,39 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="559">
@@ -4989,7 +5013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -5056,7 +5080,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -5064,7 +5088,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -5072,7 +5096,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -5086,7 +5110,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -5138,7 +5162,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="2"/>
@@ -5164,7 +5188,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="57" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="18"/>
@@ -5236,7 +5260,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="28"/>
@@ -5262,7 +5286,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="57" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="18"/>
@@ -5320,7 +5344,7 @@
         <v>10</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C22" s="6"/>
     </row>
@@ -5340,7 +5364,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="57" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="18"/>
@@ -5398,7 +5422,7 @@
         <v>10</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C32" s="6"/>
     </row>
@@ -5416,20 +5440,20 @@
       <c r="B34" s="8"/>
       <c r="C34" s="6"/>
       <c r="E34" s="70" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="57" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="18"/>
-      <c r="E35" s="86" t="s">
-        <v>78</v>
-      </c>
-      <c r="F35" s="86" t="s">
-        <v>79</v>
+      <c r="E35" s="87" t="s">
+        <v>76</v>
+      </c>
+      <c r="F35" s="87" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -5438,8 +5462,8 @@
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
-      <c r="E36" s="87"/>
-      <c r="F36" s="87"/>
+      <c r="E36" s="88"/>
+      <c r="F36" s="88"/>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="7" t="s">
@@ -5449,11 +5473,11 @@
         <v>0.9</v>
       </c>
       <c r="C37" s="6"/>
-      <c r="E37" s="88" t="s">
-        <v>80</v>
-      </c>
-      <c r="F37" s="88" t="s">
-        <v>81</v>
+      <c r="E37" s="85" t="s">
+        <v>78</v>
+      </c>
+      <c r="F37" s="85" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -5462,8 +5486,8 @@
       </c>
       <c r="B38" s="18"/>
       <c r="C38" s="6"/>
-      <c r="E38" s="89"/>
-      <c r="F38" s="89"/>
+      <c r="E38" s="86"/>
+      <c r="F38" s="86"/>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="7" t="s">
@@ -5471,11 +5495,11 @@
       </c>
       <c r="B39" s="18"/>
       <c r="C39" s="6"/>
-      <c r="E39" s="88" t="s">
-        <v>82</v>
-      </c>
-      <c r="F39" s="88" t="s">
-        <v>83</v>
+      <c r="E39" s="85" t="s">
+        <v>80</v>
+      </c>
+      <c r="F39" s="85" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -5484,81 +5508,87 @@
       </c>
       <c r="B40" s="18"/>
       <c r="C40" s="6"/>
-      <c r="E40" s="89"/>
-      <c r="F40" s="89"/>
+      <c r="E40" s="86"/>
+      <c r="F40" s="86"/>
     </row>
     <row r="41" spans="1:6">
-      <c r="E41" s="88" t="s">
+      <c r="E41" s="85" t="s">
+        <v>82</v>
+      </c>
+      <c r="F41" s="85" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="E42" s="86"/>
+      <c r="F42" s="86"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="E43" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="F41" s="88" t="s">
+      <c r="F43" s="85" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
-      <c r="E42" s="89"/>
-      <c r="F42" s="89"/>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="E43" s="88" t="s">
+    <row r="44" spans="1:6">
+      <c r="E44" s="86"/>
+      <c r="F44" s="86"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="E45" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="F43" s="88" t="s">
+      <c r="F45" s="85" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="E46" s="86"/>
+      <c r="F46" s="86"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="E47" s="85" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="E44" s="89"/>
-      <c r="F44" s="89"/>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="E45" s="88" t="s">
+      <c r="F47" s="85" t="s">
         <v>88</v>
       </c>
-      <c r="F45" s="88" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="E46" s="89"/>
-      <c r="F46" s="89"/>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="E47" s="88" t="s">
+    </row>
+    <row r="48" spans="1:6">
+      <c r="E48" s="86"/>
+      <c r="F48" s="86"/>
+    </row>
+    <row r="49" spans="5:6">
+      <c r="E49" s="85" t="s">
         <v>89</v>
       </c>
-      <c r="F47" s="88" t="s">
+      <c r="F49" s="85" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
-      <c r="E48" s="89"/>
-      <c r="F48" s="89"/>
-    </row>
-    <row r="49" spans="5:6">
-      <c r="E49" s="88" t="s">
-        <v>91</v>
-      </c>
-      <c r="F49" s="88" t="s">
-        <v>92</v>
-      </c>
-    </row>
     <row r="50" spans="5:6">
-      <c r="E50" s="89"/>
-      <c r="F50" s="89"/>
+      <c r="E50" s="86"/>
+      <c r="F50" s="86"/>
     </row>
     <row r="51" spans="5:6">
       <c r="E51" s="71" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="5:6" ht="28" customHeight="1">
       <c r="E53" s="71" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
     <mergeCell ref="E47:E48"/>
     <mergeCell ref="F47:F48"/>
     <mergeCell ref="E49:E50"/>
@@ -5569,12 +5599,6 @@
     <mergeCell ref="F43:F44"/>
     <mergeCell ref="E45:E46"/>
     <mergeCell ref="F45:F46"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5619,147 +5643,147 @@
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E1" s="13"/>
       <c r="F1" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G1" s="13"/>
       <c r="H1" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I1" s="13"/>
       <c r="J1" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K1" s="13"/>
       <c r="L1" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M1" s="13"/>
       <c r="N1" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="O1" s="13"/>
       <c r="P1" s="12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="Q1" s="13"/>
       <c r="R1" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="S1" s="13"/>
       <c r="T1" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="U1" s="13"/>
       <c r="V1" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="W1" s="13"/>
       <c r="X1" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="Y1" s="13"/>
       <c r="Z1" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AA1" s="13"/>
       <c r="AB1" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AC1" s="13"/>
       <c r="AD1" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AE1" s="13"/>
       <c r="AF1" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AG1" s="13"/>
       <c r="AH1" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="AI1" s="13"/>
       <c r="AJ1" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AK1" s="13"/>
       <c r="AL1" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="AM1" s="13"/>
       <c r="AN1" s="12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="AO1" s="13"/>
       <c r="AP1" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AQ1" s="13"/>
       <c r="AR1" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="AS1" s="13"/>
       <c r="AT1" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AU1" s="13"/>
       <c r="AV1" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AW1" s="13"/>
       <c r="AX1" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AY1" s="13"/>
       <c r="AZ1" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="BA1" s="13"/>
       <c r="BB1" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="BC1" s="13"/>
       <c r="BD1" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="BE1" s="13"/>
       <c r="BF1" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="BG1" s="13"/>
       <c r="BH1" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="BI1" s="13"/>
       <c r="BJ1" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="BK1" s="13"/>
       <c r="BL1" s="12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="BM1" s="13"/>
       <c r="BN1" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="BO1" s="13"/>
       <c r="BP1" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="BQ1" s="13"/>
       <c r="BR1" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="BS1" s="13"/>
       <c r="BT1" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="BU1" s="13"/>
       <c r="BV1" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="BW1" s="13"/>
     </row>
@@ -5990,7 +6014,7 @@
     </row>
     <row r="3" spans="1:75">
       <c r="A3" s="72" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B3" s="15">
         <v>8</v>
@@ -6368,7 +6392,7 @@
     </row>
     <row r="5" spans="1:75">
       <c r="A5" s="72" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B5" s="15">
         <v>8</v>
@@ -6520,760 +6544,760 @@
       <c r="BW5" s="16"/>
     </row>
     <row r="6" spans="1:75">
-      <c r="A6" s="80"/>
-      <c r="B6" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="82" t="s">
+      <c r="A6" s="79"/>
+      <c r="B6" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="81" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="82" t="s">
+      <c r="E6" s="81" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="82" t="s">
+      <c r="G6" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="81" t="s">
         <v>9</v>
       </c>
       <c r="L6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="82" t="s">
+      <c r="M6" s="81" t="s">
         <v>9</v>
       </c>
       <c r="N6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="P6" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q6" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="R6" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="S6" s="82" t="s">
+      <c r="O6" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q6" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="R6" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="S6" s="81" t="s">
         <v>9</v>
       </c>
       <c r="T6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="U6" s="82" t="s">
+      <c r="U6" s="81" t="s">
         <v>9</v>
       </c>
       <c r="V6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="W6" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="X6" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y6" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z6" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA6" s="82" t="s">
+      <c r="W6" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="X6" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y6" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z6" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA6" s="81" t="s">
         <v>9</v>
       </c>
       <c r="AB6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AC6" s="82" t="s">
+      <c r="AC6" s="81" t="s">
         <v>9</v>
       </c>
       <c r="AD6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AE6" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF6" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG6" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH6" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI6" s="82" t="s">
+      <c r="AE6" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF6" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG6" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH6" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI6" s="81" t="s">
         <v>9</v>
       </c>
       <c r="AJ6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AK6" s="82" t="s">
+      <c r="AK6" s="81" t="s">
         <v>9</v>
       </c>
       <c r="AL6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AM6" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="AN6" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="AO6" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="AP6" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="AQ6" s="82" t="s">
+      <c r="AM6" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="AN6" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO6" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="AP6" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ6" s="81" t="s">
         <v>9</v>
       </c>
       <c r="AR6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AS6" s="82" t="s">
+      <c r="AS6" s="81" t="s">
         <v>9</v>
       </c>
       <c r="AT6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AU6" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="AV6" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="AW6" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="AX6" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="AY6" s="82" t="s">
+      <c r="AU6" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="AV6" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW6" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="AX6" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="AY6" s="81" t="s">
         <v>9</v>
       </c>
       <c r="AZ6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BA6" s="82" t="s">
+      <c r="BA6" s="81" t="s">
         <v>9</v>
       </c>
       <c r="BB6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BC6" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="BD6" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="BE6" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="BF6" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="BG6" s="82" t="s">
+      <c r="BC6" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="BD6" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="BE6" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="BF6" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="BG6" s="81" t="s">
         <v>9</v>
       </c>
       <c r="BH6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BI6" s="82" t="s">
+      <c r="BI6" s="81" t="s">
         <v>9</v>
       </c>
       <c r="BJ6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BK6" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="BL6" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="BM6" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="BN6" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="BO6" s="82" t="s">
+      <c r="BK6" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="BL6" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="BM6" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="BN6" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="BO6" s="81" t="s">
         <v>9</v>
       </c>
       <c r="BP6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BQ6" s="82" t="s">
+      <c r="BQ6" s="81" t="s">
         <v>9</v>
       </c>
       <c r="BR6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BS6" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="BT6" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="BU6" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="BV6" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="BW6" s="82" t="s">
+      <c r="BS6" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="BT6" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="BU6" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="BV6" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="BW6" s="81" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:75">
-      <c r="A7" s="83" t="s">
-        <v>101</v>
-      </c>
-      <c r="B7" s="84">
+      <c r="A7" s="82" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="83">
         <v>8</v>
       </c>
-      <c r="C7" s="85"/>
+      <c r="C7" s="84"/>
       <c r="D7" s="69">
         <v>13</v>
       </c>
-      <c r="E7" s="85"/>
+      <c r="E7" s="84"/>
       <c r="F7" s="69">
         <v>18</v>
       </c>
-      <c r="G7" s="85"/>
+      <c r="G7" s="84"/>
       <c r="H7" s="69">
         <v>13</v>
       </c>
-      <c r="I7" s="85"/>
-      <c r="J7" s="84">
+      <c r="I7" s="84"/>
+      <c r="J7" s="83">
         <v>8</v>
       </c>
-      <c r="K7" s="85"/>
+      <c r="K7" s="84"/>
       <c r="L7" s="69">
         <v>13</v>
       </c>
-      <c r="M7" s="85"/>
+      <c r="M7" s="84"/>
       <c r="N7" s="69">
         <v>18</v>
       </c>
-      <c r="O7" s="85"/>
+      <c r="O7" s="84"/>
       <c r="P7" s="69">
         <v>13</v>
       </c>
-      <c r="Q7" s="85"/>
-      <c r="R7" s="84">
+      <c r="Q7" s="84"/>
+      <c r="R7" s="83">
         <v>8</v>
       </c>
-      <c r="S7" s="85"/>
+      <c r="S7" s="84"/>
       <c r="T7" s="69">
         <v>13</v>
       </c>
-      <c r="U7" s="85"/>
+      <c r="U7" s="84"/>
       <c r="V7" s="69">
         <v>18</v>
       </c>
-      <c r="W7" s="85"/>
+      <c r="W7" s="84"/>
       <c r="X7" s="69">
         <v>13</v>
       </c>
-      <c r="Y7" s="85"/>
-      <c r="Z7" s="84">
+      <c r="Y7" s="84"/>
+      <c r="Z7" s="83">
         <v>8</v>
       </c>
-      <c r="AA7" s="85"/>
+      <c r="AA7" s="84"/>
       <c r="AB7" s="69">
         <v>13</v>
       </c>
-      <c r="AC7" s="85"/>
+      <c r="AC7" s="84"/>
       <c r="AD7" s="69">
         <v>18</v>
       </c>
-      <c r="AE7" s="85"/>
+      <c r="AE7" s="84"/>
       <c r="AF7" s="69">
         <v>13</v>
       </c>
-      <c r="AG7" s="85"/>
-      <c r="AH7" s="84">
+      <c r="AG7" s="84"/>
+      <c r="AH7" s="83">
         <v>8</v>
       </c>
-      <c r="AI7" s="85"/>
+      <c r="AI7" s="84"/>
       <c r="AJ7" s="69">
         <v>13</v>
       </c>
-      <c r="AK7" s="85"/>
+      <c r="AK7" s="84"/>
       <c r="AL7" s="69">
         <v>18</v>
       </c>
-      <c r="AM7" s="85"/>
+      <c r="AM7" s="84"/>
       <c r="AN7" s="69">
         <v>13</v>
       </c>
-      <c r="AO7" s="85"/>
-      <c r="AP7" s="84">
+      <c r="AO7" s="84"/>
+      <c r="AP7" s="83">
         <v>8</v>
       </c>
-      <c r="AQ7" s="85"/>
+      <c r="AQ7" s="84"/>
       <c r="AR7" s="69">
         <v>13</v>
       </c>
-      <c r="AS7" s="85"/>
+      <c r="AS7" s="84"/>
       <c r="AT7" s="69">
         <v>18</v>
       </c>
-      <c r="AU7" s="85"/>
+      <c r="AU7" s="84"/>
       <c r="AV7" s="69">
         <v>13</v>
       </c>
-      <c r="AW7" s="85"/>
-      <c r="AX7" s="84">
+      <c r="AW7" s="84"/>
+      <c r="AX7" s="83">
         <v>8</v>
       </c>
-      <c r="AY7" s="85"/>
+      <c r="AY7" s="84"/>
       <c r="AZ7" s="69">
         <v>13</v>
       </c>
-      <c r="BA7" s="85"/>
+      <c r="BA7" s="84"/>
       <c r="BB7" s="69">
         <v>18</v>
       </c>
-      <c r="BC7" s="85"/>
+      <c r="BC7" s="84"/>
       <c r="BD7" s="69">
         <v>13</v>
       </c>
-      <c r="BE7" s="85"/>
-      <c r="BF7" s="84">
+      <c r="BE7" s="84"/>
+      <c r="BF7" s="83">
         <v>8</v>
       </c>
-      <c r="BG7" s="85"/>
+      <c r="BG7" s="84"/>
       <c r="BH7" s="69">
         <v>13</v>
       </c>
-      <c r="BI7" s="85"/>
+      <c r="BI7" s="84"/>
       <c r="BJ7" s="69">
         <v>18</v>
       </c>
-      <c r="BK7" s="85"/>
+      <c r="BK7" s="84"/>
       <c r="BL7" s="69">
         <v>13</v>
       </c>
-      <c r="BM7" s="85"/>
-      <c r="BN7" s="84">
+      <c r="BM7" s="84"/>
+      <c r="BN7" s="83">
         <v>8</v>
       </c>
-      <c r="BO7" s="85"/>
+      <c r="BO7" s="84"/>
       <c r="BP7" s="69">
         <v>13</v>
       </c>
-      <c r="BQ7" s="85"/>
+      <c r="BQ7" s="84"/>
       <c r="BR7" s="69">
         <v>18</v>
       </c>
-      <c r="BS7" s="85"/>
+      <c r="BS7" s="84"/>
       <c r="BT7" s="69">
         <v>13</v>
       </c>
-      <c r="BU7" s="85"/>
-      <c r="BV7" s="84">
+      <c r="BU7" s="84"/>
+      <c r="BV7" s="83">
         <v>8</v>
       </c>
-      <c r="BW7" s="85"/>
+      <c r="BW7" s="84"/>
     </row>
     <row r="8" spans="1:75">
-      <c r="A8" s="80"/>
-      <c r="B8" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="82" t="s">
+      <c r="A8" s="79"/>
+      <c r="B8" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="81" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="82" t="s">
+      <c r="E8" s="81" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="82" t="s">
+      <c r="G8" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="81" t="s">
         <v>9</v>
       </c>
       <c r="L8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="M8" s="82" t="s">
+      <c r="M8" s="81" t="s">
         <v>9</v>
       </c>
       <c r="N8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="O8" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="P8" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q8" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="R8" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="S8" s="82" t="s">
+      <c r="O8" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="P8" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q8" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="R8" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="S8" s="81" t="s">
         <v>9</v>
       </c>
       <c r="T8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="U8" s="82" t="s">
+      <c r="U8" s="81" t="s">
         <v>9</v>
       </c>
       <c r="V8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="W8" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="X8" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y8" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z8" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA8" s="82" t="s">
+      <c r="W8" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="X8" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y8" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z8" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA8" s="81" t="s">
         <v>9</v>
       </c>
       <c r="AB8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AC8" s="82" t="s">
+      <c r="AC8" s="81" t="s">
         <v>9</v>
       </c>
       <c r="AD8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AE8" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF8" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG8" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH8" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI8" s="82" t="s">
+      <c r="AE8" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF8" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG8" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH8" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI8" s="81" t="s">
         <v>9</v>
       </c>
       <c r="AJ8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AK8" s="82" t="s">
+      <c r="AK8" s="81" t="s">
         <v>9</v>
       </c>
       <c r="AL8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AM8" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="AN8" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="AO8" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="AP8" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="AQ8" s="82" t="s">
+      <c r="AM8" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="AN8" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO8" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="AP8" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ8" s="81" t="s">
         <v>9</v>
       </c>
       <c r="AR8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AS8" s="82" t="s">
+      <c r="AS8" s="81" t="s">
         <v>9</v>
       </c>
       <c r="AT8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AU8" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="AV8" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="AW8" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="AX8" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="AY8" s="82" t="s">
+      <c r="AU8" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="AV8" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW8" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="AX8" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="AY8" s="81" t="s">
         <v>9</v>
       </c>
       <c r="AZ8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BA8" s="82" t="s">
+      <c r="BA8" s="81" t="s">
         <v>9</v>
       </c>
       <c r="BB8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BC8" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="BD8" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="BE8" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="BF8" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="BG8" s="82" t="s">
+      <c r="BC8" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="BD8" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="BE8" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="BF8" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="BG8" s="81" t="s">
         <v>9</v>
       </c>
       <c r="BH8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BI8" s="82" t="s">
+      <c r="BI8" s="81" t="s">
         <v>9</v>
       </c>
       <c r="BJ8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BK8" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="BL8" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="BM8" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="BN8" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="BO8" s="82" t="s">
+      <c r="BK8" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="BL8" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="BM8" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="BN8" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="BO8" s="81" t="s">
         <v>9</v>
       </c>
       <c r="BP8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BQ8" s="82" t="s">
+      <c r="BQ8" s="81" t="s">
         <v>9</v>
       </c>
       <c r="BR8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BS8" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="BT8" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="BU8" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="BV8" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="BW8" s="82" t="s">
+      <c r="BS8" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="BT8" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="BU8" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="BV8" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="BW8" s="81" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:75">
-      <c r="A9" s="83" t="s">
-        <v>101</v>
-      </c>
-      <c r="B9" s="84">
+      <c r="A9" s="82" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="83">
         <v>8</v>
       </c>
-      <c r="C9" s="85"/>
+      <c r="C9" s="84"/>
       <c r="D9" s="69">
         <v>13</v>
       </c>
-      <c r="E9" s="85"/>
+      <c r="E9" s="84"/>
       <c r="F9" s="69">
         <v>18</v>
       </c>
-      <c r="G9" s="85"/>
+      <c r="G9" s="84"/>
       <c r="H9" s="69">
         <v>13</v>
       </c>
-      <c r="I9" s="85"/>
-      <c r="J9" s="84">
+      <c r="I9" s="84"/>
+      <c r="J9" s="83">
         <v>8</v>
       </c>
-      <c r="K9" s="85"/>
+      <c r="K9" s="84"/>
       <c r="L9" s="69">
         <v>13</v>
       </c>
-      <c r="M9" s="85"/>
+      <c r="M9" s="84"/>
       <c r="N9" s="69">
         <v>18</v>
       </c>
-      <c r="O9" s="85"/>
+      <c r="O9" s="84"/>
       <c r="P9" s="69">
         <v>13</v>
       </c>
-      <c r="Q9" s="85"/>
-      <c r="R9" s="84">
+      <c r="Q9" s="84"/>
+      <c r="R9" s="83">
         <v>8</v>
       </c>
-      <c r="S9" s="85"/>
+      <c r="S9" s="84"/>
       <c r="T9" s="69">
         <v>13</v>
       </c>
-      <c r="U9" s="85"/>
+      <c r="U9" s="84"/>
       <c r="V9" s="69">
         <v>18</v>
       </c>
-      <c r="W9" s="85"/>
+      <c r="W9" s="84"/>
       <c r="X9" s="69">
         <v>13</v>
       </c>
-      <c r="Y9" s="85"/>
-      <c r="Z9" s="84">
+      <c r="Y9" s="84"/>
+      <c r="Z9" s="83">
         <v>8</v>
       </c>
-      <c r="AA9" s="85"/>
+      <c r="AA9" s="84"/>
       <c r="AB9" s="69">
         <v>13</v>
       </c>
-      <c r="AC9" s="85"/>
+      <c r="AC9" s="84"/>
       <c r="AD9" s="69">
         <v>18</v>
       </c>
-      <c r="AE9" s="85"/>
+      <c r="AE9" s="84"/>
       <c r="AF9" s="69">
         <v>13</v>
       </c>
-      <c r="AG9" s="85"/>
-      <c r="AH9" s="84">
+      <c r="AG9" s="84"/>
+      <c r="AH9" s="83">
         <v>8</v>
       </c>
-      <c r="AI9" s="85"/>
+      <c r="AI9" s="84"/>
       <c r="AJ9" s="69">
         <v>13</v>
       </c>
-      <c r="AK9" s="85"/>
+      <c r="AK9" s="84"/>
       <c r="AL9" s="69">
         <v>18</v>
       </c>
-      <c r="AM9" s="85"/>
+      <c r="AM9" s="84"/>
       <c r="AN9" s="69">
         <v>13</v>
       </c>
-      <c r="AO9" s="85"/>
-      <c r="AP9" s="84">
+      <c r="AO9" s="84"/>
+      <c r="AP9" s="83">
         <v>8</v>
       </c>
-      <c r="AQ9" s="85"/>
+      <c r="AQ9" s="84"/>
       <c r="AR9" s="69">
         <v>13</v>
       </c>
-      <c r="AS9" s="85"/>
+      <c r="AS9" s="84"/>
       <c r="AT9" s="69">
         <v>18</v>
       </c>
-      <c r="AU9" s="85"/>
+      <c r="AU9" s="84"/>
       <c r="AV9" s="69">
         <v>13</v>
       </c>
-      <c r="AW9" s="85"/>
-      <c r="AX9" s="84">
+      <c r="AW9" s="84"/>
+      <c r="AX9" s="83">
         <v>8</v>
       </c>
-      <c r="AY9" s="85"/>
+      <c r="AY9" s="84"/>
       <c r="AZ9" s="69">
         <v>13</v>
       </c>
-      <c r="BA9" s="85"/>
+      <c r="BA9" s="84"/>
       <c r="BB9" s="69">
         <v>18</v>
       </c>
-      <c r="BC9" s="85"/>
+      <c r="BC9" s="84"/>
       <c r="BD9" s="69">
         <v>13</v>
       </c>
-      <c r="BE9" s="85"/>
-      <c r="BF9" s="84">
+      <c r="BE9" s="84"/>
+      <c r="BF9" s="83">
         <v>8</v>
       </c>
-      <c r="BG9" s="85"/>
+      <c r="BG9" s="84"/>
       <c r="BH9" s="69">
         <v>13</v>
       </c>
-      <c r="BI9" s="85"/>
+      <c r="BI9" s="84"/>
       <c r="BJ9" s="69">
         <v>18</v>
       </c>
-      <c r="BK9" s="85"/>
+      <c r="BK9" s="84"/>
       <c r="BL9" s="69">
         <v>13</v>
       </c>
-      <c r="BM9" s="85"/>
-      <c r="BN9" s="84">
+      <c r="BM9" s="84"/>
+      <c r="BN9" s="83">
         <v>8</v>
       </c>
-      <c r="BO9" s="85"/>
+      <c r="BO9" s="84"/>
       <c r="BP9" s="69">
         <v>13</v>
       </c>
-      <c r="BQ9" s="85"/>
+      <c r="BQ9" s="84"/>
       <c r="BR9" s="69">
         <v>18</v>
       </c>
-      <c r="BS9" s="85"/>
+      <c r="BS9" s="84"/>
       <c r="BT9" s="69">
         <v>13</v>
       </c>
-      <c r="BU9" s="85"/>
-      <c r="BV9" s="84">
+      <c r="BU9" s="84"/>
+      <c r="BV9" s="83">
         <v>8</v>
       </c>
-      <c r="BW9" s="85"/>
+      <c r="BW9" s="84"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7291,8 +7315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7329,8 +7353,8 @@
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="42" t="s">
-        <v>112</v>
+      <c r="B2" s="89" t="s">
+        <v>110</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="28"/>
@@ -7349,7 +7373,7 @@
       <c r="A3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="42">
+      <c r="B3" s="89">
         <v>6.36</v>
       </c>
       <c r="C3" s="6"/>
@@ -7369,7 +7393,7 @@
       <c r="A4" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="43"/>
+      <c r="B4" s="90"/>
       <c r="C4" s="6"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
@@ -7387,7 +7411,7 @@
       <c r="A5" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="42"/>
+      <c r="B5" s="89"/>
       <c r="C5" s="6"/>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
@@ -7403,7 +7427,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="9" t="s">
-        <v>71</v>
+        <v>154</v>
       </c>
       <c r="B6" s="42">
         <v>2.2400000000000002</v>
@@ -7423,7 +7447,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="69" t="s">
-        <v>72</v>
+        <v>155</v>
       </c>
       <c r="B7" s="43">
         <v>0.1</v>
@@ -7443,7 +7467,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="5" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="B8" s="42"/>
       <c r="C8" s="6"/>
@@ -7460,8 +7484,8 @@
       <c r="N8" s="28"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="19" t="s">
-        <v>143</v>
+      <c r="A9" s="5" t="s">
+        <v>157</v>
       </c>
       <c r="B9" s="42"/>
       <c r="C9" s="42"/>
@@ -7478,11 +7502,9 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B10" s="79">
-        <v>5.0000000000000004E-6</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="B10" s="91"/>
       <c r="C10" s="6"/>
       <c r="D10" s="28"/>
       <c r="E10" s="28"/>
@@ -7497,11 +7519,9 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="B11" s="8">
-        <v>2.65E-5</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="B11" s="89"/>
       <c r="C11" s="6"/>
       <c r="D11" s="28"/>
       <c r="E11" s="28"/>
@@ -7515,10 +7535,10 @@
       <c r="M11" s="28"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B12" s="42"/>
+      <c r="A12" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" s="92"/>
       <c r="C12" s="6"/>
       <c r="D12" s="28"/>
       <c r="E12" s="28"/>
@@ -7532,10 +7552,12 @@
       <c r="M12" s="28"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="B13" s="42"/>
+      <c r="A13" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" s="93">
+        <v>5.0000000000000004E-6</v>
+      </c>
       <c r="C13" s="42"/>
       <c r="D13" s="28"/>
       <c r="E13" s="28"/>
@@ -7551,96 +7573,108 @@
     </row>
     <row r="14" spans="1:14" ht="18" customHeight="1">
       <c r="A14" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B14" s="79">
-        <v>5.0000000000000004E-6</v>
+        <v>159</v>
+      </c>
+      <c r="B14" s="94">
+        <v>2.65E-5</v>
       </c>
       <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="B15" s="8">
-        <v>2.65E-5</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="B15" s="89"/>
       <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B16" s="42"/>
+      <c r="A16" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" s="89"/>
+      <c r="C16" s="6"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="B17" s="42"/>
+      <c r="A17" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" s="93">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:3" ht="17" customHeight="1">
       <c r="A18" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B18" s="8">
-        <v>6.3999999999999997E-6</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="B18" s="94">
+        <v>2.65E-5</v>
+      </c>
+      <c r="C18" s="6"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B19" s="8">
-        <v>1.2500000000000001E-5</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="B19" s="89"/>
+      <c r="C19" s="6"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B20" s="42"/>
-      <c r="C20" s="2"/>
+      <c r="A20" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" s="89"/>
+      <c r="C20" s="42"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="B21" s="42"/>
-      <c r="C21" s="2"/>
+      <c r="A21" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B21" s="94">
+        <v>6.3999999999999997E-6</v>
+      </c>
+      <c r="C21" s="6"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="B22" s="8">
-        <v>6.3999999999999997E-6</v>
-      </c>
-      <c r="C22" s="2"/>
+        <v>148</v>
+      </c>
+      <c r="B22" s="94">
+        <v>1.2500000000000001E-5</v>
+      </c>
+      <c r="C22" s="6"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="B23" s="8">
+        <v>137</v>
+      </c>
+      <c r="B23" s="89"/>
+      <c r="C23" s="42"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="B24" s="89"/>
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B25" s="94">
+        <v>6.3999999999999997E-6</v>
+      </c>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B26" s="94">
         <v>1.2500000000000001E-5</v>
       </c>
-      <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="56"/>
-      <c r="C26" s="2"/>
+      <c r="C26" s="6"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="58"/>
@@ -7770,7 +7804,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="23" t="s">
@@ -7795,7 +7829,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B3" s="6">
         <v>4.7E-2</v>
@@ -7814,7 +7848,7 @@
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K3" s="36">
         <v>0.08</v>
@@ -8033,7 +8067,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="2"/>
@@ -8042,7 +8076,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B15" s="6">
         <v>9.8000000000000004E-2</v>
@@ -8160,13 +8194,13 @@
         <v>10</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C26" s="6"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B27" s="6">
         <v>0.43099999999999999</v>
@@ -8283,7 +8317,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="53" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B2" s="53"/>
     </row>
@@ -8313,7 +8347,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="53" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B6" s="53">
         <v>0</v>
@@ -8321,7 +8355,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="53" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B7" s="53">
         <v>0</v>
@@ -8332,7 +8366,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="53" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B8" s="53">
         <v>0</v>
@@ -8348,7 +8382,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="53" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B10" s="53"/>
     </row>
@@ -8378,7 +8412,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="53" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B14" s="53">
         <v>0</v>
@@ -8386,7 +8420,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="53" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B15" s="53">
         <v>0</v>
@@ -8394,7 +8428,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="53" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B16" s="53">
         <v>0</v>
@@ -8413,7 +8447,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="53" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B18" s="53"/>
     </row>
@@ -8443,7 +8477,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="53" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B22" s="53">
         <v>0.7</v>
@@ -8451,7 +8485,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="53" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B23" s="53">
         <v>0</v>
@@ -8462,7 +8496,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="53" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B24" s="53">
         <v>0</v>
@@ -8551,34 +8585,34 @@
         <v>63</v>
       </c>
       <c r="E1" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="H1" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="G1" s="44" t="s">
+      <c r="I1" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="H1" s="44" t="s">
+      <c r="J1" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="I1" s="44" t="s">
-        <v>121</v>
-      </c>
-      <c r="J1" s="44" t="s">
-        <v>122</v>
-      </c>
       <c r="K1" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="L1" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="M1" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="L1" s="44" t="s">
+      <c r="N1" s="44" t="s">
         <v>120</v>
-      </c>
-      <c r="M1" s="44" t="s">
-        <v>121</v>
-      </c>
-      <c r="N1" s="44" t="s">
-        <v>122</v>
       </c>
       <c r="O1" s="44" t="s">
         <v>38</v>
@@ -8590,34 +8624,34 @@
         <v>63</v>
       </c>
       <c r="R1" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="S1" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="T1" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="S1" s="44" t="s">
+      <c r="U1" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="T1" s="44" t="s">
+      <c r="V1" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="U1" s="44" t="s">
+      <c r="W1" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="V1" s="44" t="s">
-        <v>121</v>
-      </c>
-      <c r="W1" s="44" t="s">
-        <v>122</v>
-      </c>
       <c r="X1" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y1" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="Z1" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="Y1" s="44" t="s">
+      <c r="AA1" s="44" t="s">
         <v>120</v>
-      </c>
-      <c r="Z1" s="44" t="s">
-        <v>121</v>
-      </c>
-      <c r="AA1" s="44" t="s">
-        <v>122</v>
       </c>
       <c r="AB1" s="44" t="s">
         <v>38</v>
@@ -8629,34 +8663,34 @@
         <v>63</v>
       </c>
       <c r="AE1" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="AF1" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG1" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="AF1" s="44" t="s">
+      <c r="AH1" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="AG1" s="44" t="s">
+      <c r="AI1" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="AH1" s="44" t="s">
+      <c r="AJ1" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="AI1" s="44" t="s">
-        <v>121</v>
-      </c>
-      <c r="AJ1" s="44" t="s">
-        <v>122</v>
-      </c>
       <c r="AK1" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL1" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="AM1" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="AL1" s="44" t="s">
+      <c r="AN1" s="44" t="s">
         <v>120</v>
-      </c>
-      <c r="AM1" s="44" t="s">
-        <v>121</v>
-      </c>
-      <c r="AN1" s="44" t="s">
-        <v>122</v>
       </c>
       <c r="AO1" s="44" t="s">
         <v>38</v>
@@ -8668,34 +8702,34 @@
         <v>63</v>
       </c>
       <c r="AR1" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="AS1" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="AT1" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="AS1" s="44" t="s">
+      <c r="AU1" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="AT1" s="44" t="s">
+      <c r="AV1" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="AU1" s="44" t="s">
+      <c r="AW1" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="AV1" s="44" t="s">
-        <v>121</v>
-      </c>
-      <c r="AW1" s="44" t="s">
-        <v>122</v>
-      </c>
       <c r="AX1" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="AY1" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="AZ1" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="AY1" s="44" t="s">
+      <c r="BA1" s="44" t="s">
         <v>120</v>
-      </c>
-      <c r="AZ1" s="44" t="s">
-        <v>121</v>
-      </c>
-      <c r="BA1" s="44" t="s">
-        <v>122</v>
       </c>
       <c r="BB1" s="17"/>
       <c r="BC1" s="17"/>
@@ -9179,7 +9213,7 @@
     </row>
     <row r="2" spans="1:532">
       <c r="A2" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B2" s="45">
         <v>1</v>
@@ -9344,7 +9378,7 @@
     </row>
     <row r="3" spans="1:532">
       <c r="A3" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B3" s="45">
         <v>1</v>
@@ -9509,7 +9543,7 @@
     </row>
     <row r="4" spans="1:532">
       <c r="A4" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B4" s="45">
         <v>1</v>
@@ -9729,13 +9763,13 @@
         <v>45</v>
       </c>
       <c r="C2" s="47" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="47" t="s">
         <v>123</v>
-      </c>
-      <c r="D2" s="47" t="s">
-        <v>124</v>
-      </c>
-      <c r="E2" s="47" t="s">
-        <v>125</v>
       </c>
       <c r="F2" s="17"/>
       <c r="G2" s="17"/>
@@ -9760,10 +9794,10 @@
     <row r="4" spans="1:8">
       <c r="A4" s="48"/>
       <c r="B4" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
@@ -9774,10 +9808,10 @@
     <row r="5" spans="1:8">
       <c r="A5" s="48"/>
       <c r="B5" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -9788,10 +9822,10 @@
     <row r="6" spans="1:8">
       <c r="A6" s="48"/>
       <c r="B6" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
@@ -9802,10 +9836,10 @@
     <row r="7" spans="1:8">
       <c r="A7" s="48"/>
       <c r="B7" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" s="48" t="s">
         <v>133</v>
-      </c>
-      <c r="C7" s="48" t="s">
-        <v>135</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
@@ -10143,13 +10177,13 @@
     </row>
     <row r="40" spans="1:49">
       <c r="A40" s="45" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B40" s="45" t="s">
         <v>49</v>
       </c>
       <c r="C40" s="45" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D40" s="51" t="s">
         <v>52</v>
@@ -10167,10 +10201,10 @@
     </row>
     <row r="41" spans="1:49">
       <c r="A41" s="45" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B41" s="45" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C41" s="45">
         <v>1</v>
@@ -10179,13 +10213,13 @@
         <v>45</v>
       </c>
       <c r="E41" s="45" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F41" s="45" t="s">
         <v>56</v>
       </c>
       <c r="G41" s="45" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H41" s="17"/>
       <c r="AW41" t="s">
@@ -10194,10 +10228,10 @@
     </row>
     <row r="42" spans="1:49">
       <c r="A42" s="45" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B42" s="46" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C42" s="45">
         <v>1</v>
@@ -10206,13 +10240,13 @@
         <v>45</v>
       </c>
       <c r="E42" s="45" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F42" s="45" t="s">
         <v>56</v>
       </c>
       <c r="G42" s="45" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H42" s="17"/>
       <c r="AW42" t="s">
@@ -10221,10 +10255,10 @@
     </row>
     <row r="43" spans="1:49">
       <c r="A43" s="46" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B43" s="46" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C43" s="46">
         <v>1</v>
@@ -10233,13 +10267,13 @@
         <v>45</v>
       </c>
       <c r="E43" s="45" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F43" s="45" t="s">
         <v>56</v>
       </c>
       <c r="G43" s="45" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AW43" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
added multiple chemicals to concentration sheet
</commit_message>
<xml_diff>
--- a/sheets/input/Pegan_Cove_South_Pond.xlsx
+++ b/sheets/input/Pegan_Cove_South_Pond.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sample and Time Input" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="139">
   <si>
     <t xml:space="preserve">Sampling Variables Inputs</t>
   </si>
@@ -72,7 +72,7 @@
     <t xml:space="preserve">Steady State</t>
   </si>
   <si>
-    <t xml:space="preserve">YES</t>
+    <t xml:space="preserve">NO</t>
   </si>
   <si>
     <t xml:space="preserve">Region</t>
@@ -260,7 +260,13 @@
     <t xml:space="preserve">Concentration in Pore Water (ug/L)</t>
   </si>
   <si>
+    <t xml:space="preserve">Concentration in Pore Water (ug/L) </t>
+  </si>
+  <si>
     <t xml:space="preserve">Pegan Cove Dummy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concentration in Pore Water (ug/L) *</t>
   </si>
   <si>
     <t xml:space="preserve">South Pond Dummy</t>
@@ -1227,9 +1233,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1017360</xdr:colOff>
+      <xdr:colOff>1017000</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>187560</xdr:rowOff>
+      <xdr:rowOff>187200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1239,7 +1245,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14045040" y="571680"/>
-          <a:ext cx="9469440" cy="7807320"/>
+          <a:ext cx="9469080" cy="7806960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1706,9 +1712,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2968200</xdr:colOff>
+      <xdr:colOff>2967840</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>73080</xdr:rowOff>
+      <xdr:rowOff>72720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1718,7 +1724,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11978640" y="546120"/>
-          <a:ext cx="2968200" cy="568800"/>
+          <a:ext cx="2967840" cy="568440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1929,9 +1935,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>5213160</xdr:colOff>
+      <xdr:colOff>5212800</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>187560</xdr:rowOff>
+      <xdr:rowOff>187200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1941,7 +1947,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11979000" y="2464920"/>
-          <a:ext cx="9910440" cy="4176720"/>
+          <a:ext cx="9910080" cy="4176360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2240,9 +2246,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>2329560</xdr:colOff>
+      <xdr:colOff>2329200</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>135000</xdr:rowOff>
+      <xdr:rowOff>134640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2256,7 +2262,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16676280" y="10278720"/>
-          <a:ext cx="2329560" cy="733680"/>
+          <a:ext cx="2329200" cy="733320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2417,9 +2423,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>239040</xdr:colOff>
+      <xdr:colOff>238680</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>174960</xdr:rowOff>
+      <xdr:rowOff>174600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2429,7 +2435,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="22839480" y="2082960"/>
-          <a:ext cx="3746160" cy="758880"/>
+          <a:ext cx="3745800" cy="758520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2559,9 +2565,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>1017000</xdr:colOff>
+      <xdr:colOff>1016640</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>32040</xdr:rowOff>
+      <xdr:rowOff>31680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2571,7 +2577,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="21425760" y="2130480"/>
-          <a:ext cx="2878560" cy="758880"/>
+          <a:ext cx="2878200" cy="758520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2913,9 +2919,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>99360</xdr:colOff>
+      <xdr:colOff>99000</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>122040</xdr:rowOff>
+      <xdr:rowOff>121680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2925,7 +2931,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="15024240" y="594720"/>
-          <a:ext cx="4075920" cy="950040"/>
+          <a:ext cx="4075560" cy="949680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2982,9 +2988,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>897120</xdr:colOff>
+      <xdr:colOff>896760</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>149400</xdr:rowOff>
+      <xdr:rowOff>149040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2994,7 +3000,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14243040" y="3772800"/>
-          <a:ext cx="9086400" cy="3476880"/>
+          <a:ext cx="9086040" cy="3476520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3442,7 +3448,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>57240</xdr:colOff>
+      <xdr:colOff>56880</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>98640</xdr:rowOff>
     </xdr:to>
@@ -3454,7 +3460,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2901600" y="9163440"/>
-          <a:ext cx="8330760" cy="650520"/>
+          <a:ext cx="8330400" cy="650520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3612,9 +3618,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>4549320</xdr:colOff>
+      <xdr:colOff>4548960</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>99360</xdr:rowOff>
+      <xdr:rowOff>99000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3624,7 +3630,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11780280" y="3467880"/>
-          <a:ext cx="4061160" cy="747360"/>
+          <a:ext cx="4060800" cy="747000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3726,9 +3732,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4613760</xdr:colOff>
+      <xdr:colOff>4613400</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>140040</xdr:rowOff>
+      <xdr:rowOff>139680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3738,7 +3744,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17375400" y="3725640"/>
-          <a:ext cx="4330440" cy="339840"/>
+          <a:ext cx="4330080" cy="339480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3855,9 +3861,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>5382000</xdr:colOff>
+      <xdr:colOff>5381640</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>136800</xdr:rowOff>
+      <xdr:rowOff>136440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3867,7 +3873,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9213840" y="76320"/>
-          <a:ext cx="5254920" cy="1495440"/>
+          <a:ext cx="5254560" cy="1495080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4069,9 +4075,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>4988520</xdr:colOff>
+      <xdr:colOff>4988160</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>111600</xdr:rowOff>
+      <xdr:rowOff>111240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4081,7 +4087,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12084120" y="2705040"/>
-          <a:ext cx="1991160" cy="657720"/>
+          <a:ext cx="1990800" cy="657360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4188,9 +4194,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>759240</xdr:colOff>
+      <xdr:colOff>758880</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>149400</xdr:rowOff>
+      <xdr:rowOff>149040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4200,7 +4206,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11168280" y="4140000"/>
-          <a:ext cx="10732320" cy="390600"/>
+          <a:ext cx="10731960" cy="390240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4312,9 +4318,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>200160</xdr:colOff>
+      <xdr:colOff>199800</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>162360</xdr:rowOff>
+      <xdr:rowOff>162000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4324,7 +4330,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12163680" y="2984400"/>
-          <a:ext cx="9177840" cy="416160"/>
+          <a:ext cx="9177480" cy="415800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4381,9 +4387,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>530640</xdr:colOff>
+      <xdr:colOff>530280</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>60840</xdr:rowOff>
+      <xdr:rowOff>60480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4393,7 +4399,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12151080" y="3556080"/>
-          <a:ext cx="11885760" cy="695520"/>
+          <a:ext cx="11885400" cy="695160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4455,9 +4461,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>276480</xdr:colOff>
+      <xdr:colOff>276120</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>162360</xdr:rowOff>
+      <xdr:rowOff>162000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4467,7 +4473,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13899240" y="761760"/>
-          <a:ext cx="6528960" cy="5877360"/>
+          <a:ext cx="6528600" cy="5877000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4583,8 +4589,8 @@
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="1" sqref="L2:M5 B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4702,7 +4708,7 @@
   <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="L2:M5 A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5124,8 +5130,8 @@
   </sheetPr>
   <dimension ref="A1:BI5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2:M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5406,6 +5412,30 @@
       <c r="E2" s="0" t="n">
         <v>15</v>
       </c>
+      <c r="F2" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
@@ -5423,6 +5453,30 @@
       <c r="E3" s="0" t="n">
         <v>15</v>
       </c>
+      <c r="F3" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="s">
@@ -5440,6 +5494,30 @@
       <c r="E4" s="0" t="n">
         <v>15</v>
       </c>
+      <c r="F4" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="24" t="s">
@@ -5455,6 +5533,30 @@
         <v>15</v>
       </c>
       <c r="E5" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="M5" s="0" t="n">
         <v>15</v>
       </c>
     </row>
@@ -5478,7 +5580,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="1" sqref="L2:M5 B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5665,7 +5767,7 @@
   <dimension ref="A1:BJ45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="1" sqref="L2:M5 B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6648,7 +6750,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="39" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B12" s="42" t="n">
         <v>2.65E-005</v>
@@ -6836,7 +6938,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="43" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7166,7 +7268,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="39" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B18" s="42" t="n">
         <v>2.65E-005</v>
@@ -8595,7 +8697,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="45" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9402,7 +9504,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
+      <selection pane="topLeft" activeCell="A38" activeCellId="1" sqref="L2:M5 A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9424,25 +9526,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="46" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B1" s="46" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D1" s="46" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="47" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F1" s="46" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="46" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H1" s="48" t="s">
         <v>16</v>
@@ -9454,7 +9556,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C2" s="50" t="s">
         <v>17</v>
@@ -9464,34 +9566,34 @@
         <v>17</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H2" s="52" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="50" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B3" s="12" t="n">
         <v>0.047</v>
       </c>
       <c r="C3" s="50" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D3" s="53"/>
       <c r="E3" s="50" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F3" s="53" t="n">
         <v>5.7E-008</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H3" s="53" t="n">
         <v>0.08</v>
@@ -9499,23 +9601,23 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="50" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B4" s="12" t="n">
         <v>0.037</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D4" s="52"/>
       <c r="E4" s="50" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F4" s="52" t="n">
         <v>0.031</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H4" s="52" t="n">
         <v>0.012</v>
@@ -9523,21 +9625,21 @@
     </row>
     <row r="5" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="50" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="50" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D5" s="52"/>
       <c r="E5" s="50" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F5" s="52" t="n">
         <v>0.047</v>
       </c>
       <c r="G5" s="30" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H5" s="52" t="n">
         <v>0.02</v>
@@ -9546,105 +9648,105 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="50" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B6" s="17"/>
       <c r="C6" s="50" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="50" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="50" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B7" s="54"/>
       <c r="C7" s="50" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="50" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F7" s="12"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="50" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B8" s="54"/>
       <c r="C8" s="50" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="50" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F8" s="12"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="50" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B9" s="52"/>
       <c r="C9" s="50" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="50" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B10" s="55"/>
       <c r="C10" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="50" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F10" s="12"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B11" s="52"/>
       <c r="C11" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D11" s="56"/>
       <c r="E11" s="50" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F11" s="56"/>
     </row>
     <row r="12" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B12" s="56"/>
       <c r="C12" s="57" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D12" s="58"/>
       <c r="E12" s="50" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F12" s="59" t="n">
         <v>0</v>
@@ -9652,22 +9754,22 @@
     </row>
     <row r="13" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="46" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B13" s="46" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9675,7 +9777,7 @@
         <v>17</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -9683,7 +9785,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="50" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B15" s="12" t="n">
         <v>0.098</v>
@@ -9694,7 +9796,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="50" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B16" s="12" t="n">
         <v>0.0202</v>
@@ -9705,7 +9807,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="50" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B17" s="12"/>
       <c r="D17" s="5"/>
@@ -9714,7 +9816,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="50" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B18" s="17"/>
       <c r="D18" s="5"/>
@@ -9723,7 +9825,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="50" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B19" s="54"/>
       <c r="D19" s="5"/>
@@ -9732,7 +9834,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="50" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B20" s="54"/>
       <c r="D20" s="5"/>
@@ -9741,7 +9843,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="50" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B21" s="52"/>
       <c r="D21" s="5"/>
@@ -9750,7 +9852,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B22" s="55"/>
       <c r="D22" s="5"/>
@@ -9759,7 +9861,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B23" s="52"/>
       <c r="D23" s="5"/>
@@ -9768,7 +9870,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B24" s="56"/>
       <c r="D24" s="5"/>
@@ -9777,7 +9879,7 @@
     </row>
     <row r="25" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="46" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B25" s="46" t="s">
         <v>16</v>
@@ -9788,12 +9890,12 @@
         <v>17</v>
       </c>
       <c r="B26" s="51" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="50" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B27" s="12" t="n">
         <v>0.431</v>
@@ -9801,7 +9903,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="50" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B28" s="12" t="n">
         <v>0.0276</v>
@@ -9809,58 +9911,58 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="50" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B29" s="12"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="50" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B30" s="17"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="50" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B31" s="54"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="50" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B32" s="54"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="50" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B33" s="52"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B34" s="55"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B35" s="52"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B36" s="56"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -9883,7 +9985,7 @@
   <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="1" sqref="L2:M5 C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9899,18 +10001,18 @@
         <v>16</v>
       </c>
       <c r="B1" s="64" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="65" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B2" s="65"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="65" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B3" s="65" t="n">
         <v>0</v>
@@ -9918,7 +10020,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="65" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B4" s="65" t="n">
         <v>0.6</v>
@@ -9926,7 +10028,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="65" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B5" s="65" t="n">
         <v>0.4</v>
@@ -9934,7 +10036,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="65" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B6" s="65" t="n">
         <v>0</v>
@@ -9942,7 +10044,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="65" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B7" s="65" t="n">
         <v>0</v>
@@ -9953,7 +10055,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="65" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B8" s="65" t="n">
         <v>0</v>
@@ -9964,18 +10066,18 @@
         <v>16</v>
       </c>
       <c r="B9" s="64" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="65" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B10" s="65"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="65" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B11" s="65" t="n">
         <v>0</v>
@@ -9983,7 +10085,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="65" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B12" s="65" t="n">
         <v>0.2</v>
@@ -9991,7 +10093,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="65" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B13" s="65" t="n">
         <v>0.8</v>
@@ -9999,7 +10101,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="65" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B14" s="65" t="n">
         <v>0</v>
@@ -10007,7 +10109,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="65" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B15" s="65" t="n">
         <v>0</v>
@@ -10015,7 +10117,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="65" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B16" s="65" t="n">
         <v>0</v>
@@ -10029,18 +10131,18 @@
         <v>16</v>
       </c>
       <c r="B17" s="64" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="65" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B18" s="65"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="65" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B19" s="65" t="n">
         <v>0</v>
@@ -10048,7 +10150,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="65" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B20" s="65" t="n">
         <v>0.1</v>
@@ -10056,7 +10158,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="65" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B21" s="65" t="n">
         <v>0.2</v>
@@ -10064,7 +10166,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="65" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B22" s="65" t="n">
         <v>0.7</v>
@@ -10072,7 +10174,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="65" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B23" s="65" t="n">
         <v>0</v>
@@ -10083,7 +10185,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="65" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B24" s="65" t="n">
         <v>0</v>
@@ -10131,7 +10233,7 @@
   <dimension ref="A1:TL4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB1" activeCellId="0" sqref="AB1"/>
+      <selection pane="topLeft" activeCell="AB1" activeCellId="1" sqref="L2:M5 AB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10166,163 +10268,163 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="V1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AO1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="X1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AX1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AB1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="AZ1" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="BB1" s="27"/>
       <c r="BC1" s="27"/>
@@ -10806,7 +10908,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="66" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B2" s="67" t="n">
         <v>1</v>
@@ -10971,7 +11073,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="66" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B3" s="67" t="n">
         <v>1</v>
@@ -11136,7 +11238,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="66" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B4" s="67" t="n">
         <v>1</v>
@@ -11318,8 +11420,8 @@
   </sheetPr>
   <dimension ref="A1:AW100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="1" sqref="L2:M5 A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11336,19 +11438,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F1" s="27"/>
       <c r="G1" s="27"/>
@@ -11357,16 +11459,16 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12"/>
       <c r="B2" s="12" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F2" s="27"/>
       <c r="G2" s="27"/>
@@ -11374,13 +11476,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D3" s="27"/>
       <c r="E3" s="27"/>
@@ -11394,7 +11496,7 @@
         <v>18</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D4" s="27"/>
       <c r="E4" s="27"/>
@@ -11408,7 +11510,7 @@
         <v>27</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D5" s="27"/>
       <c r="E5" s="27"/>
@@ -11422,7 +11524,7 @@
         <v>28</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="27"/>
@@ -11436,7 +11538,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="27"/>
@@ -11756,16 +11858,16 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="70" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B39" s="70" t="n">
         <v>40</v>
       </c>
       <c r="C39" s="70" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D39" s="70" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E39" s="27"/>
       <c r="F39" s="27"/>
@@ -11774,106 +11876,106 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="67" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B40" s="67" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C40" s="67" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D40" s="71" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E40" s="71" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F40" s="71" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G40" s="71" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H40" s="72"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="67" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B41" s="67" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C41" s="67" t="n">
         <v>1</v>
       </c>
       <c r="D41" s="67" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E41" s="67" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F41" s="67" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G41" s="67" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H41" s="27"/>
       <c r="AW41" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="67" t="s">
+        <v>137</v>
+      </c>
+      <c r="B42" s="68" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="E42" s="67" t="s">
+        <v>134</v>
+      </c>
+      <c r="F42" s="67" t="s">
         <v>135</v>
       </c>
-      <c r="B42" s="68" t="s">
-        <v>92</v>
-      </c>
-      <c r="C42" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="D42" s="67" t="s">
-        <v>110</v>
-      </c>
-      <c r="E42" s="67" t="s">
-        <v>132</v>
-      </c>
-      <c r="F42" s="67" t="s">
-        <v>133</v>
-      </c>
       <c r="G42" s="67" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H42" s="27"/>
       <c r="AW42" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="B43" s="68" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="D43" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="E43" s="67" t="s">
+        <v>134</v>
+      </c>
+      <c r="F43" s="67" t="s">
+        <v>135</v>
+      </c>
+      <c r="G43" s="67" t="s">
         <v>136</v>
       </c>
-      <c r="B43" s="68" t="s">
-        <v>93</v>
-      </c>
-      <c r="C43" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="D43" s="67" t="s">
-        <v>110</v>
-      </c>
-      <c r="E43" s="67" t="s">
-        <v>132</v>
-      </c>
-      <c r="F43" s="67" t="s">
-        <v>133</v>
-      </c>
-      <c r="G43" s="67" t="s">
-        <v>134</v>
-      </c>
       <c r="AW43" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11885,7 +11987,7 @@
       <c r="F44" s="68"/>
       <c r="G44" s="68"/>
       <c r="AW44" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11897,7 +11999,7 @@
       <c r="F45" s="68"/>
       <c r="G45" s="68"/>
       <c r="AW45" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11909,7 +12011,7 @@
       <c r="F46" s="68"/>
       <c r="G46" s="68"/>
       <c r="AW46" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11921,7 +12023,7 @@
       <c r="F47" s="68"/>
       <c r="G47" s="68"/>
       <c r="AW47" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11933,7 +12035,7 @@
       <c r="F48" s="68"/>
       <c r="G48" s="68"/>
       <c r="AW48" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11945,7 +12047,7 @@
       <c r="F49" s="68"/>
       <c r="G49" s="68"/>
       <c r="AW49" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11957,7 +12059,7 @@
       <c r="F50" s="68"/>
       <c r="G50" s="68"/>
       <c r="AW50" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11969,7 +12071,7 @@
       <c r="F51" s="68"/>
       <c r="G51" s="68"/>
       <c r="AW51" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11981,7 +12083,7 @@
       <c r="F52" s="68"/>
       <c r="G52" s="68"/>
       <c r="AW52" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11993,7 +12095,7 @@
       <c r="F53" s="68"/>
       <c r="G53" s="68"/>
       <c r="AW53" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12005,7 +12107,7 @@
       <c r="F54" s="68"/>
       <c r="G54" s="68"/>
       <c r="AW54" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12017,7 +12119,7 @@
       <c r="F55" s="68"/>
       <c r="G55" s="68"/>
       <c r="AW55" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12029,231 +12131,231 @@
       <c r="F56" s="68"/>
       <c r="G56" s="68"/>
       <c r="AW56" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW57" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW58" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW59" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW60" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW61" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW62" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW63" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW64" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW65" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW66" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW67" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW68" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW69" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW70" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW71" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW72" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW73" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW74" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW75" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW76" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW77" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW78" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW79" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW80" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW81" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW82" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW83" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW84" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW85" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW86" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW87" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW88" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW89" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW90" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW91" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW92" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW93" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW94" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW95" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW96" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW97" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW98" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AW99" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="27"/>
       <c r="B100" s="27" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="AW100" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed some bugs, but am not working on prior concentrations, bug for pcsp
</commit_message>
<xml_diff>
--- a/sheets/input/Pegan_Cove_South_Pond.xlsx
+++ b/sheets/input/Pegan_Cove_South_Pond.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sample and Time Input" sheetId="1" state="visible" r:id="rId2"/>
@@ -171,7 +171,6 @@
         <color rgb="FF333333"/>
         <rFont val="OpenSans"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">λ, </t>
     </r>
@@ -182,7 +181,6 @@
         <color rgb="FF333333"/>
         <rFont val="OpenSans"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">k </t>
     </r>
@@ -476,13 +474,12 @@
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="31">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -498,6 +495,77 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -539,7 +607,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -547,7 +614,6 @@
       <color rgb="FF333333"/>
       <name val="OpenSans"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -555,14 +621,12 @@
       <color rgb="FF333333"/>
       <name val="OpenSans"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="OpenSans"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -570,7 +634,6 @@
       <color rgb="FF333333"/>
       <name val="OpenSans"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -588,14 +651,12 @@
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -603,12 +664,54 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="29">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFDDE0E2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFFAC090"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF948A54"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFDDE0E2"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -667,7 +770,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF7B59"/>
-        <bgColor rgb="FFFF6600"/>
+        <bgColor rgb="FFDA9694"/>
       </patternFill>
     </fill>
     <fill>
@@ -709,7 +812,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF948A54"/>
-        <bgColor rgb="FF808000"/>
+        <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
     <fill>
@@ -731,12 +834,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -832,7 +950,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -856,25 +974,76 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="73">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -882,87 +1051,87 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="12" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="13" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="16" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="16" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="19" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="12" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -970,59 +1139,59 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="13" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="20" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="21" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="22" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="23" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="16" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="23" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1030,71 +1199,71 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="17" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="24" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="15" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="22" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="24" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="18" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="25" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="18" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="25" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="25" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="29" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="13" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="6" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="13" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1102,89 +1271,106 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="17" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="10" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="17" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="19" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="26" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="20" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="27" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="20" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="27" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="21" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="28" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="20" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="27" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Heading" xfId="20"/>
+    <cellStyle name="Heading 1" xfId="21"/>
+    <cellStyle name="Heading 2" xfId="22"/>
+    <cellStyle name="Text" xfId="23"/>
+    <cellStyle name="Note" xfId="24"/>
+    <cellStyle name="Footnote" xfId="25"/>
+    <cellStyle name="Hyperlink" xfId="26"/>
+    <cellStyle name="Status" xfId="27"/>
+    <cellStyle name="Good" xfId="28"/>
+    <cellStyle name="Neutral" xfId="29"/>
+    <cellStyle name="Bad" xfId="30"/>
+    <cellStyle name="Warning" xfId="31"/>
+    <cellStyle name="Error" xfId="32"/>
+    <cellStyle name="Accent" xfId="33"/>
+    <cellStyle name="Accent 1" xfId="34"/>
+    <cellStyle name="Accent 2" xfId="35"/>
+    <cellStyle name="Accent 3" xfId="36"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF0000EE"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC4BD97"/>
-      <rgbColor rgb="FF948A54"/>
+      <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF8EB4E3"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFAFD095"/>
+      <rgbColor rgb="FFDDE0E2"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF7B59"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDE0E2"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFF200"/>
@@ -1194,21 +1380,21 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFC4D79B"/>
-      <rgbColor rgb="FFC3D69B"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF93CDDD"/>
       <rgbColor rgb="FFFFA6A6"/>
       <rgbColor rgb="FFB3A2C7"/>
       <rgbColor rgb="FFFAC090"/>
       <rgbColor rgb="FF538DD5"/>
-      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FFAFD095"/>
       <rgbColor rgb="FF81D41A"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFC3D69B"/>
       <rgbColor rgb="FFDA9694"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFD99694"/>
       <rgbColor rgb="FF5585B8"/>
-      <rgbColor rgb="FFD99694"/>
+      <rgbColor rgb="FF948A54"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF558ED5"/>
       <rgbColor rgb="FF003300"/>
@@ -1227,15 +1413,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
+      <xdr:colOff>1080</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1017000</xdr:colOff>
+      <xdr:colOff>1017360</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>187200</xdr:rowOff>
+      <xdr:rowOff>186840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1244,8 +1430,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14045040" y="571680"/>
-          <a:ext cx="9469080" cy="7806960"/>
+          <a:off x="14045760" y="572400"/>
+          <a:ext cx="9468720" cy="7805880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1712,9 +1898,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2967840</xdr:colOff>
+      <xdr:colOff>2967480</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>72720</xdr:rowOff>
+      <xdr:rowOff>73080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1724,7 +1910,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11978640" y="546120"/>
-          <a:ext cx="2967840" cy="568440"/>
+          <a:ext cx="2967480" cy="568800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1822,15 +2008,9 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -1867,15 +2047,9 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -1912,15 +2086,9 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -1935,9 +2103,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>5212800</xdr:colOff>
+      <xdr:colOff>5212440</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>187200</xdr:rowOff>
+      <xdr:rowOff>186840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1947,7 +2115,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11979000" y="2464920"/>
-          <a:ext cx="9910080" cy="4176360"/>
+          <a:ext cx="9909720" cy="4176000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2246,9 +2414,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>2329200</xdr:colOff>
+      <xdr:colOff>2328840</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>134640</xdr:rowOff>
+      <xdr:rowOff>134280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2262,7 +2430,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16676280" y="10278720"/>
-          <a:ext cx="2329200" cy="733320"/>
+          <a:ext cx="2328840" cy="732960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2310,15 +2478,9 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -2355,15 +2517,9 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -2400,15 +2556,9 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -2419,13 +2569,13 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>572040</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>178920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>238680</xdr:colOff>
+      <xdr:colOff>239040</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>174600</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2434,8 +2584,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="22839480" y="2082960"/>
-          <a:ext cx="3745800" cy="758520"/>
+          <a:off x="22839480" y="2083680"/>
+          <a:ext cx="3746160" cy="757440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2520,7 +2670,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>89280</xdr:colOff>
+      <xdr:colOff>89640</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>12600</xdr:rowOff>
     </xdr:to>
@@ -2532,7 +2682,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="22534920" y="3632040"/>
-          <a:ext cx="2881080" cy="0"/>
+          <a:ext cx="2881440" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2542,15 +2692,9 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -2561,13 +2705,13 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>178200</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>35280</xdr:rowOff>
+      <xdr:rowOff>36000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>1016640</xdr:colOff>
+      <xdr:colOff>1016280</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>31680</xdr:rowOff>
+      <xdr:rowOff>32040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2576,8 +2720,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="21425760" y="2130480"/>
-          <a:ext cx="2878200" cy="758520"/>
+          <a:off x="21425760" y="2131200"/>
+          <a:ext cx="2877840" cy="758160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2671,15 +2815,9 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -2716,15 +2854,9 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -2761,15 +2893,9 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -2806,15 +2932,9 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -2851,15 +2971,9 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -2896,15 +3010,9 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -2913,15 +3021,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1383480</xdr:colOff>
+      <xdr:colOff>1384200</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>124200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>99000</xdr:colOff>
+      <xdr:colOff>99360</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>121680</xdr:rowOff>
+      <xdr:rowOff>122040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2930,8 +3038,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15024240" y="594720"/>
-          <a:ext cx="4075560" cy="949680"/>
+          <a:off x="15024960" y="594720"/>
+          <a:ext cx="4075200" cy="950040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2982,15 +3090,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>602280</xdr:colOff>
+      <xdr:colOff>603000</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>101520</xdr:rowOff>
+      <xdr:rowOff>102240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>896760</xdr:colOff>
+      <xdr:colOff>897120</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>149040</xdr:rowOff>
+      <xdr:rowOff>149400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2999,8 +3107,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14243040" y="3772800"/>
-          <a:ext cx="9086040" cy="3476520"/>
+          <a:off x="14243760" y="3773520"/>
+          <a:ext cx="9085680" cy="3476160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3448,7 +3556,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>56880</xdr:colOff>
+      <xdr:colOff>56520</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>98640</xdr:rowOff>
     </xdr:to>
@@ -3460,7 +3568,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2901600" y="9163440"/>
-          <a:ext cx="8330400" cy="650520"/>
+          <a:ext cx="8330040" cy="650520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3567,13 +3675,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1955880</xdr:colOff>
+      <xdr:colOff>1956240</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>142560</xdr:rowOff>
+      <xdr:rowOff>142920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1955880</xdr:colOff>
+      <xdr:colOff>1956240</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>12600</xdr:rowOff>
     </xdr:to>
@@ -3584,8 +3692,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19047960" y="3496320"/>
-          <a:ext cx="0" cy="1394280"/>
+          <a:off x="19048320" y="3496680"/>
+          <a:ext cx="0" cy="1393920"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3595,15 +3703,9 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -3614,13 +3716,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>488160</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:rowOff>114840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>4548960</xdr:colOff>
+      <xdr:colOff>4548600</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>99000</xdr:rowOff>
+      <xdr:rowOff>99360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3629,8 +3731,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11780280" y="3467880"/>
-          <a:ext cx="4060800" cy="747000"/>
+          <a:off x="11780280" y="3468600"/>
+          <a:ext cx="4060440" cy="746640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3683,13 +3785,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1562040</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1562040</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>61200</xdr:rowOff>
+      <xdr:rowOff>61560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3698,7 +3800,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="25150320" y="3163680"/>
+          <a:off x="25150320" y="3164040"/>
           <a:ext cx="0" cy="1394280"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -3709,15 +3811,9 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -3726,15 +3822,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>283320</xdr:colOff>
+      <xdr:colOff>284040</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>181080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4613400</xdr:colOff>
+      <xdr:colOff>4613760</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>139680</xdr:rowOff>
+      <xdr:rowOff>139320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3743,8 +3839,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17375400" y="3725640"/>
-          <a:ext cx="4330080" cy="339480"/>
+          <a:off x="17376120" y="3725640"/>
+          <a:ext cx="4329720" cy="339120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3805,15 +3901,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2426040</xdr:colOff>
+      <xdr:colOff>2426400</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>155160</xdr:rowOff>
+      <xdr:rowOff>155520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2426040</xdr:colOff>
+      <xdr:colOff>2426400</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>25560</xdr:rowOff>
+      <xdr:rowOff>25920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3822,7 +3918,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19518120" y="7027560"/>
+          <a:off x="19518480" y="7027920"/>
           <a:ext cx="0" cy="1394280"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -3833,15 +3929,9 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -3861,9 +3951,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>5381640</xdr:colOff>
+      <xdr:colOff>5381280</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>136440</xdr:rowOff>
+      <xdr:rowOff>148320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3873,7 +3963,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9213840" y="76320"/>
-          <a:ext cx="5254560" cy="1495080"/>
+          <a:ext cx="5254200" cy="1494720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3936,13 +4026,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>1955520</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>139680</xdr:rowOff>
+      <xdr:rowOff>163800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2781000</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>149760</xdr:rowOff>
+      <xdr:rowOff>173880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3962,15 +4052,9 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -3981,13 +4065,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>2781000</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>149760</xdr:rowOff>
+      <xdr:rowOff>173880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2781360</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>88560</xdr:rowOff>
+      <xdr:rowOff>112680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4007,15 +4091,9 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -4026,13 +4104,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>1955520</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>88560</xdr:rowOff>
+      <xdr:rowOff>112680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2781000</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>88920</xdr:rowOff>
+      <xdr:rowOff>113040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4052,15 +4130,9 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -4071,13 +4143,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>2997360</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>25560</xdr:rowOff>
+      <xdr:rowOff>50400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>4988160</xdr:colOff>
+      <xdr:colOff>4987800</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>111240</xdr:rowOff>
+      <xdr:rowOff>135000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4086,8 +4158,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12084120" y="2705040"/>
-          <a:ext cx="1990800" cy="657360"/>
+          <a:off x="12084120" y="2705760"/>
+          <a:ext cx="1990440" cy="656280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4143,15 +4215,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>444240</xdr:colOff>
+      <xdr:colOff>444600</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>25200</xdr:rowOff>
+      <xdr:rowOff>25560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1287720</xdr:colOff>
+      <xdr:colOff>1288080</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>30240</xdr:rowOff>
+      <xdr:rowOff>30600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4160,7 +4232,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9986760" y="3263400"/>
+          <a:off x="9987120" y="3263760"/>
           <a:ext cx="843480" cy="5040"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -4171,15 +4243,9 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -4188,15 +4254,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1625760</xdr:colOff>
+      <xdr:colOff>1626480</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>139680</xdr:rowOff>
+      <xdr:rowOff>140400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>758880</xdr:colOff>
+      <xdr:colOff>759240</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>149040</xdr:rowOff>
+      <xdr:rowOff>149400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4205,8 +4271,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11168280" y="4140000"/>
-          <a:ext cx="10731960" cy="390240"/>
+          <a:off x="11169000" y="4140720"/>
+          <a:ext cx="10731600" cy="389880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4267,13 +4333,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>75960</xdr:colOff>
+      <xdr:colOff>76320</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>37800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>75960</xdr:colOff>
+      <xdr:colOff>76320</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>139680</xdr:rowOff>
     </xdr:to>
@@ -4284,7 +4350,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11820600" y="3466800"/>
+          <a:off x="11820960" y="3466800"/>
           <a:ext cx="0" cy="1435320"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -4295,15 +4361,9 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -4312,15 +4372,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>419040</xdr:colOff>
+      <xdr:colOff>419760</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>127080</xdr:rowOff>
+      <xdr:rowOff>127800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>199800</xdr:colOff>
+      <xdr:colOff>200160</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:rowOff>162360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4329,8 +4389,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12163680" y="2984400"/>
-          <a:ext cx="9177480" cy="415800"/>
+          <a:off x="12164400" y="2985120"/>
+          <a:ext cx="9177120" cy="415440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4381,15 +4441,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>406440</xdr:colOff>
+      <xdr:colOff>407160</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>127080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>530280</xdr:colOff>
+      <xdr:colOff>530640</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>60480</xdr:rowOff>
+      <xdr:rowOff>60840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4398,8 +4458,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12151080" y="3556080"/>
-          <a:ext cx="11885400" cy="695160"/>
+          <a:off x="12151800" y="3556080"/>
+          <a:ext cx="11885040" cy="695520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4455,15 +4515,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>406440</xdr:colOff>
+      <xdr:colOff>407160</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>276120</xdr:colOff>
+      <xdr:colOff>275760</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:rowOff>162360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4472,8 +4532,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13899240" y="761760"/>
-          <a:ext cx="6528600" cy="5877000"/>
+          <a:off x="13899960" y="762480"/>
+          <a:ext cx="6527520" cy="5876640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4590,7 +4650,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="1" sqref="L2:M5 B10"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4708,7 +4768,7 @@
   <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="L2:M5 A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5130,8 +5190,8 @@
   </sheetPr>
   <dimension ref="A1:BI5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2:M5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5580,7 +5640,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="1" sqref="L2:M5 B12"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5766,8 +5826,8 @@
   </sheetPr>
   <dimension ref="A1:BJ45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="1" sqref="L2:M5 B18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9504,7 +9564,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A38" activeCellId="1" sqref="L2:M5 A38"/>
+      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9985,7 +10045,7 @@
   <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="1" sqref="L2:M5 C11"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9996,7 +10056,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.49"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="63" t="s">
         <v>16</v>
       </c>
@@ -10061,7 +10121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="23" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="63" t="s">
         <v>16</v>
       </c>
@@ -10126,7 +10186,7 @@
       <c r="I16" s="27"/>
       <c r="J16" s="27"/>
     </row>
-    <row r="17" customFormat="false" ht="23" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="63" t="s">
         <v>16</v>
       </c>
@@ -10233,7 +10293,7 @@
   <dimension ref="A1:TL4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB1" activeCellId="1" sqref="L2:M5 AB1"/>
+      <selection pane="topLeft" activeCell="AB1" activeCellId="0" sqref="AB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11421,7 +11481,7 @@
   <dimension ref="A1:AW100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="1" sqref="L2:M5 A10"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
caught the space error in coordinates
</commit_message>
<xml_diff>
--- a/sheets/input/Pegan_Cove_South_Pond.xlsx
+++ b/sheets/input/Pegan_Cove_South_Pond.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Sample and Time Input" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="140">
   <si>
     <t xml:space="preserve">Sampling Variables Inputs</t>
   </si>
@@ -171,6 +171,7 @@
         <color rgb="FF333333"/>
         <rFont val="OpenSans"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">λ, </t>
     </r>
@@ -181,6 +182,7 @@
         <color rgb="FF333333"/>
         <rFont val="OpenSans"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">k </t>
     </r>
@@ -384,16 +386,16 @@
     <t xml:space="preserve">Coordinate 4</t>
   </si>
   <si>
-    <t xml:space="preserve">0,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20,20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20,0</t>
+    <t xml:space="preserve">0, 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0, 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20, 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20, 0</t>
   </si>
   <si>
     <t xml:space="preserve">Sites:</t>
@@ -405,16 +407,19 @@
     <t xml:space="preserve">(x,y) (meters)</t>
   </si>
   <si>
-    <t xml:space="preserve">5,15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15,15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15,5</t>
+    <t xml:space="preserve">5, 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5, 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15, 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15, 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">Number of Regional Samples per Fish Population :</t>
@@ -450,13 +455,13 @@
     <t xml:space="preserve">dummy pumpkin</t>
   </si>
   <si>
-    <t xml:space="preserve">0,10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,0</t>
+    <t xml:space="preserve">0, 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10, 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10, 0</t>
   </si>
   <si>
     <t xml:space="preserve">dummy bluegill</t>
@@ -480,6 +485,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -497,23 +503,34 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
-      <sz val="24"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF333333"/>
+      <color rgb="FFCC0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -521,6 +538,29 @@
       <color rgb="FF808080"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -528,44 +568,21 @@
       <color rgb="FF0000EE"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFCC0000"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -607,6 +624,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -614,6 +632,7 @@
       <color rgb="FF333333"/>
       <name val="OpenSans"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -621,12 +640,14 @@
       <color rgb="FF333333"/>
       <name val="OpenSans"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="OpenSans"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -634,6 +655,7 @@
       <color rgb="FF333333"/>
       <name val="OpenSans"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -651,12 +673,14 @@
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -673,13 +697,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF948A54"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFDDE0E2"/>
       </patternFill>
     </fill>
@@ -697,20 +727,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFDDE0E2"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF948A54"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFDDE0E2"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -974,10 +998,46 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -986,43 +1046,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -1327,23 +1351,23 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Heading" xfId="20"/>
-    <cellStyle name="Heading 1" xfId="21"/>
-    <cellStyle name="Heading 2" xfId="22"/>
-    <cellStyle name="Text" xfId="23"/>
-    <cellStyle name="Note" xfId="24"/>
-    <cellStyle name="Footnote" xfId="25"/>
-    <cellStyle name="Hyperlink" xfId="26"/>
-    <cellStyle name="Status" xfId="27"/>
-    <cellStyle name="Good" xfId="28"/>
-    <cellStyle name="Neutral" xfId="29"/>
-    <cellStyle name="Bad" xfId="30"/>
-    <cellStyle name="Warning" xfId="31"/>
-    <cellStyle name="Error" xfId="32"/>
-    <cellStyle name="Accent" xfId="33"/>
-    <cellStyle name="Accent 1" xfId="34"/>
-    <cellStyle name="Accent 2" xfId="35"/>
-    <cellStyle name="Accent 3" xfId="36"/>
+    <cellStyle name="Accent 1 17" xfId="20"/>
+    <cellStyle name="Accent 16" xfId="21"/>
+    <cellStyle name="Accent 2 18" xfId="22"/>
+    <cellStyle name="Accent 3 19" xfId="23"/>
+    <cellStyle name="Bad 13" xfId="24"/>
+    <cellStyle name="Error 15" xfId="25"/>
+    <cellStyle name="Footnote 8" xfId="26"/>
+    <cellStyle name="Good 11" xfId="27"/>
+    <cellStyle name="Heading 1 4" xfId="28"/>
+    <cellStyle name="Heading 2 5" xfId="29"/>
+    <cellStyle name="Heading 3" xfId="30"/>
+    <cellStyle name="Hyperlink 9" xfId="31"/>
+    <cellStyle name="Neutral 12" xfId="32"/>
+    <cellStyle name="Note 7" xfId="33"/>
+    <cellStyle name="Status 10" xfId="34"/>
+    <cellStyle name="Text 6" xfId="35"/>
+    <cellStyle name="Warning 14" xfId="36"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1419,9 +1443,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1017360</xdr:colOff>
+      <xdr:colOff>1017000</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>186840</xdr:rowOff>
+      <xdr:rowOff>186480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1431,7 +1455,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14045760" y="572400"/>
-          <a:ext cx="9468720" cy="7805880"/>
+          <a:ext cx="9468360" cy="7805520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1898,9 +1922,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2967480</xdr:colOff>
+      <xdr:colOff>2967120</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>73080</xdr:rowOff>
+      <xdr:rowOff>72720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1910,7 +1934,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11978640" y="546120"/>
-          <a:ext cx="2967480" cy="568800"/>
+          <a:ext cx="2967120" cy="568440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2103,9 +2127,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>5212440</xdr:colOff>
+      <xdr:colOff>5212080</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>186840</xdr:rowOff>
+      <xdr:rowOff>186480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2115,7 +2139,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11979000" y="2464920"/>
-          <a:ext cx="9909720" cy="4176000"/>
+          <a:ext cx="9909360" cy="4175640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2414,9 +2438,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>2328840</xdr:colOff>
+      <xdr:colOff>2328480</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>134280</xdr:rowOff>
+      <xdr:rowOff>133920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2430,7 +2454,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16676280" y="10278720"/>
-          <a:ext cx="2328840" cy="732960"/>
+          <a:ext cx="2328480" cy="732600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2573,9 +2597,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>239040</xdr:colOff>
+      <xdr:colOff>238680</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2585,7 +2609,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="22839480" y="2083680"/>
-          <a:ext cx="3746160" cy="757440"/>
+          <a:ext cx="3745800" cy="757080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2709,9 +2733,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>1016280</xdr:colOff>
+      <xdr:colOff>1015920</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>32040</xdr:rowOff>
+      <xdr:rowOff>31680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2721,7 +2745,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="21425760" y="2131200"/>
-          <a:ext cx="2877840" cy="758160"/>
+          <a:ext cx="2877480" cy="757800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3027,9 +3051,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>99360</xdr:colOff>
+      <xdr:colOff>99000</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>122040</xdr:rowOff>
+      <xdr:rowOff>121680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3039,7 +3063,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="15024960" y="594720"/>
-          <a:ext cx="4075200" cy="950040"/>
+          <a:ext cx="4074840" cy="949680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3096,9 +3120,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>897120</xdr:colOff>
+      <xdr:colOff>896760</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>149400</xdr:rowOff>
+      <xdr:rowOff>149040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3108,7 +3132,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14243760" y="3773520"/>
-          <a:ext cx="9085680" cy="3476160"/>
+          <a:ext cx="9085320" cy="3475800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3556,7 +3580,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>56520</xdr:colOff>
+      <xdr:colOff>56160</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>98640</xdr:rowOff>
     </xdr:to>
@@ -3568,7 +3592,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2901600" y="9163440"/>
-          <a:ext cx="8330040" cy="650520"/>
+          <a:ext cx="8329680" cy="650520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3720,9 +3744,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>4548600</xdr:colOff>
+      <xdr:colOff>4548240</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>99360</xdr:rowOff>
+      <xdr:rowOff>99000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3732,7 +3756,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11780280" y="3468600"/>
-          <a:ext cx="4060440" cy="746640"/>
+          <a:ext cx="4060080" cy="746280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3828,9 +3852,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4613760</xdr:colOff>
+      <xdr:colOff>4613400</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>139320</xdr:rowOff>
+      <xdr:rowOff>138960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3840,7 +3864,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17376120" y="3725640"/>
-          <a:ext cx="4329720" cy="339120"/>
+          <a:ext cx="4329360" cy="338760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3951,9 +3975,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>5381280</xdr:colOff>
+      <xdr:colOff>5380920</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>148320</xdr:rowOff>
+      <xdr:rowOff>147960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3963,7 +3987,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9213840" y="76320"/>
-          <a:ext cx="5254200" cy="1494720"/>
+          <a:ext cx="5253840" cy="1494360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4147,9 +4171,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>4987800</xdr:colOff>
+      <xdr:colOff>4987440</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>135000</xdr:rowOff>
+      <xdr:rowOff>134640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4159,7 +4183,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12084120" y="2705760"/>
-          <a:ext cx="1990440" cy="656280"/>
+          <a:ext cx="1990080" cy="655920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4260,9 +4284,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>759240</xdr:colOff>
+      <xdr:colOff>758880</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>149400</xdr:rowOff>
+      <xdr:rowOff>149040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4272,7 +4296,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11169000" y="4140720"/>
-          <a:ext cx="10731600" cy="389880"/>
+          <a:ext cx="10731240" cy="389520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4378,9 +4402,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>200160</xdr:colOff>
+      <xdr:colOff>199800</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>162360</xdr:rowOff>
+      <xdr:rowOff>162000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4390,7 +4414,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12164400" y="2985120"/>
-          <a:ext cx="9177120" cy="415440"/>
+          <a:ext cx="9176760" cy="415080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4447,9 +4471,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>530640</xdr:colOff>
+      <xdr:colOff>530280</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>60840</xdr:rowOff>
+      <xdr:rowOff>60480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4459,7 +4483,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12151800" y="3556080"/>
-          <a:ext cx="11885040" cy="695520"/>
+          <a:ext cx="11884680" cy="695160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4521,9 +4545,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>275760</xdr:colOff>
+      <xdr:colOff>275400</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>162360</xdr:rowOff>
+      <xdr:rowOff>162000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4533,7 +4557,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13899960" y="762480"/>
-          <a:ext cx="6527520" cy="5876640"/>
+          <a:ext cx="6527160" cy="5876280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5826,7 +5850,7 @@
   </sheetPr>
   <dimension ref="A1:BJ45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -11480,8 +11504,8 @@
   </sheetPr>
   <dimension ref="A1:AW100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G44" activeCellId="0" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11609,7 +11633,9 @@
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="D8" s="27"/>
       <c r="E8" s="27"/>
       <c r="F8" s="27"/>
@@ -11918,16 +11944,16 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="70" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B39" s="70" t="n">
         <v>40</v>
       </c>
       <c r="C39" s="70" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D39" s="70" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E39" s="27"/>
       <c r="F39" s="27"/>
@@ -11936,31 +11962,31 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="67" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B40" s="67" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C40" s="67" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D40" s="71" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E40" s="71" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F40" s="71" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G40" s="71" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H40" s="72"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="67" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B41" s="67" t="s">
         <v>78</v>
@@ -11972,13 +11998,13 @@
         <v>112</v>
       </c>
       <c r="E41" s="67" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F41" s="67" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G41" s="67" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H41" s="27"/>
       <c r="AW41" s="0" t="s">
@@ -11987,7 +12013,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="67" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B42" s="68" t="s">
         <v>94</v>
@@ -11999,13 +12025,13 @@
         <v>112</v>
       </c>
       <c r="E42" s="67" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F42" s="67" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G42" s="67" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H42" s="27"/>
       <c r="AW42" s="0" t="s">
@@ -12014,7 +12040,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="68" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B43" s="68" t="s">
         <v>95</v>
@@ -12026,13 +12052,13 @@
         <v>112</v>
       </c>
       <c r="E43" s="67" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F43" s="67" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G43" s="67" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AW43" s="0" t="s">
         <v>87</v>

</xml_diff>